<commit_message>
v0.0.16.7 xlsx 3 safe_one
</commit_message>
<xml_diff>
--- a/ERapp/static/Kizeo.xlsx
+++ b/ERapp/static/Kizeo.xlsx
@@ -655,7 +655,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -665,17 +665,20 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI Semibold"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI Semibold"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI Semibold"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -693,11 +696,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI Semibold"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Segoe UI Semibold"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -710,26 +715,19 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI Semibold"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <name val="Segoe UI Semibold"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -794,7 +792,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -836,17 +834,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -1026,6 +1013,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1096,30 +1129,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1129,179 +1169,168 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1391,15 +1420,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>214</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1762125" cy="1333500"/>
+    <xdr:ext cx="2143125" cy="1619250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="c97373f905977pu614513_20231009000754_1558.jpg">
+        <xdr:cNvPr id="13" name="c97373f905977pu614513_20231008231119_1530.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
@@ -1426,15 +1455,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>249</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1771650" cy="1333500"/>
+    <xdr:ext cx="1762125" cy="1333500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="c97373f905977pu614513_20231009000908_1560.jpg">
+        <xdr:cNvPr id="15" name="c97373f905977pu614513_20231008231325_1540.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
@@ -1461,15 +1490,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>259</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1771650" cy="1333500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="c97373f905977pu614513_20231009001051_1562.jpg">
+        <xdr:cNvPr id="17" name="c97373f905977pu614513_20231008231402_1542.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
@@ -1496,15 +1525,15 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>270</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1762125" cy="1333500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="c97373f905977pu614513_20231009001353_1564.jpg">
+        <xdr:cNvPr id="19" name="c97373f905977pu614513_20231008231441_1544.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
@@ -1533,13 +1562,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>214</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2143125" cy="1619250"/>
+    <xdr:ext cx="1762125" cy="1333500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="c97373f905977pu614513_20231008231119_1530.jpg">
+        <xdr:cNvPr id="23" name="c97373f905977pu614513_20231009001651_1572.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
@@ -1568,13 +1597,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>249</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1762125" cy="1333500"/>
+    <xdr:ext cx="1771650" cy="1333500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="c97373f905977pu614513_20231008231325_1540.jpg">
+        <xdr:cNvPr id="25" name="c97373f905977pu614513_20231009001928_1574.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
@@ -1603,13 +1632,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>259</xdr:row>
+      <xdr:row>130</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1771650" cy="1333500"/>
+    <xdr:ext cx="1762125" cy="1333500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="c97373f905977pu614513_20231008231402_1542.jpg">
+        <xdr:cNvPr id="27" name="c97373f905977pu614513_20231008231838_1546.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
@@ -1638,13 +1667,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>270</xdr:row>
+      <xdr:row>146</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1762125" cy="1333500"/>
+    <xdr:ext cx="1771650" cy="1333500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="c97373f905977pu614513_20231008231441_1544.jpg">
+        <xdr:cNvPr id="29" name="c97373f905977pu614513_20231008232002_1552.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
@@ -1673,13 +1702,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>159</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1771650" cy="1333500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="c97373f905977pu614513_20231009001522_1566.jpg">
+        <xdr:cNvPr id="31" name="c97373f905977pu614513_20231008232204_1554.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19"/>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
@@ -1708,13 +1737,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>173</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1762125" cy="1333500"/>
+    <xdr:ext cx="1724025" cy="1333500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="c97373f905977pu614513_20231009001651_1572.jpg">
+        <xdr:cNvPr id="33" name="c97373f905977pu614513_20231008232757_1558.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21"/>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
@@ -1743,13 +1772,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>185</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1771650" cy="1333500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="c97373f905977pu614513_20231009001928_1574.jpg">
+        <xdr:cNvPr id="35" name="c97373f905977pu614513_20231008233225_1560.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23"/>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
@@ -1778,13 +1807,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>130</xdr:row>
+      <xdr:row>197</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1762125" cy="1333500"/>
+    <xdr:ext cx="1533525" cy="1333500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="c97373f905977pu614513_20231008231838_1546.jpg">
+        <xdr:cNvPr id="37" name="c97373f905977pu614513_20231008233328_1562.jpg">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25"/>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
@@ -1793,181 +1822,6 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>146</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1771650" cy="1333500"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="c97373f905977pu614513_20231008232002_1552.jpg">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27"/>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>159</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1771650" cy="1333500"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="c97373f905977pu614513_20231008232204_1554.jpg">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29"/>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>173</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1724025" cy="1333500"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="c97373f905977pu614513_20231008232757_1558.jpg">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31"/>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>185</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1771650" cy="1333500"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="c97373f905977pu614513_20231008233225_1560.jpg">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33"/>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>197</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1533525" cy="1333500"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="c97373f905977pu614513_20231008233328_1562.jpg">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId35"/>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2277,7 +2131,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,10 +2148,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="26"/>
     </row>
     <row r="2" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2429,7 +2283,7 @@
   <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2444,31 +2298,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="28" t="s">
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="T1" s="35" t="s">
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="T1" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
     </row>
     <row r="2" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="11" t="s">
         <v>30</v>
       </c>
@@ -2499,10 +2353,10 @@
       <c r="M2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="30" t="s">
+      <c r="N2" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="31"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="13" t="s">
         <v>34</v>
       </c>
@@ -2529,10 +2383,10 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="23" t="s">
         <v>46</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -2576,10 +2430,10 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="23" t="s">
         <v>52</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -2629,10 +2483,10 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="23" t="s">
         <v>58</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -2676,10 +2530,10 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="23" t="s">
         <v>62</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -2735,10 +2589,10 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="23" t="s">
         <v>65</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -2788,10 +2642,10 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="23" t="s">
         <v>70</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -2835,10 +2689,10 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="23" t="s">
         <v>72</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -2888,10 +2742,10 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="3" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="23" t="s">
         <v>75</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -2941,10 +2795,10 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="23" t="s">
         <v>76</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -2988,10 +2842,10 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="3" t="s">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="23" t="s">
         <v>77</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -3041,10 +2895,10 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="23" t="s">
         <v>78</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -3088,10 +2942,10 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="23" t="s">
         <v>79</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -3141,10 +2995,10 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="23" t="s">
         <v>80</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -3188,10 +3042,10 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="3" t="s">
         <v>47</v>
       </c>
@@ -3235,31 +3089,6 @@
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="T1:W1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUmdPcnE5allSUHgyVElGWU94VzZMam9oRUZDSncvM1pUVWR3ZFdHYmxGOW89?name="/>
-    <hyperlink ref="A4" r:id="rId2" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUmtQeFdYTCt6RnhESDJXdlhGQVZTZUZLazZxbktVYWY5NzJPMllVVXFmUW89?name="/>
-    <hyperlink ref="A5" r:id="rId3" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUmozZDl2ZVhrcGhUSUxybnBxeTdjcmFzMVFVaDBQcElsQXdHSUM5cEtrRDQ9?name="/>
-    <hyperlink ref="A6" r:id="rId4" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUjg4WmFXbFVTS2FBaEhLZmc1VUkwTDcrcjNpbkx1TC9kYW1ranBLUDIvcFk9?name="/>
-    <hyperlink ref="A7" r:id="rId5" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUnhZOGxic1JuR3JpdmpPMjhDWll6U2dyKy9za3Z3NVE4L2NzN2JRMGFmbWc9?name="/>
-    <hyperlink ref="A8" r:id="rId6" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUlMvbksyL0l0MnRVaXJNTG80WWJQOG5ENjhGN0p6Mi8wYTRoYzFOWFg2dms9?name="/>
-    <hyperlink ref="A9" r:id="rId7" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUklMeklpUnd3VDVUeG5YY2p2S29mdFlFRmJFRW1jWUpmWUJsQVl5WGVCaEk9?name="/>
-    <hyperlink ref="A10" r:id="rId8" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUkZRYWxud0xha2Rjb3FOYTk5RE8zVktTNDEvNGRLdGNLWWFodE5vdzcyT1k9?name="/>
-    <hyperlink ref="A11" r:id="rId9" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUkNaUmx6eStRVzlDVnhKai8reDVLa0ZOR282NFE4dTFhajRJOXl2aVBGb0U9?name="/>
-    <hyperlink ref="A12" r:id="rId10" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUkpKZW41cDJXMjM0UUx6VFl6NC9tSEFIVlpFZWFDcHVTdmFodGFkdjBEcG89?name="/>
-    <hyperlink ref="A14" r:id="rId11" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUk1uUnlkT0pzZEhSMFF1Z2pIZU85Y0EwWVdGeW1yQzhsYldOS3FMd0QyS289?name="/>
-    <hyperlink ref="A15" r:id="rId12" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUkJUb1RoOUxYSmllU0pSclphbmhjUFRvRUxVa084V1hUUkNMc0N0SjhldU09?name="/>
-    <hyperlink ref="B4" r:id="rId13" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUnBhOTcyVS9aSHhhaE1rdkJOeXhlMGZLU2kwV0JtbkRtbU4wVUhlRXpCcTg9?name="/>
-    <hyperlink ref="B5" r:id="rId14" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUmozZDl2ZVhrcGhUSUxybnBxeTdjclh1NXptUzdwZk5Ic2F3ZnVmSDd3K0E9?name="/>
-    <hyperlink ref="B6" r:id="rId15" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUjg4WmFXbFVTS2FBaEhLZmc1VUkwTDZsRnE0OC8zTE9aR05SR2dnMXVCL2c9?name="/>
-    <hyperlink ref="B7" r:id="rId16" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUlF3aExPU1c1dGhUUDd6SW5wQ3U4WmpCQXhHRWNPWFN5OVJmdUFwRXZyUVU9?name="/>
-    <hyperlink ref="B9" r:id="rId17" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUklMeklpUnd3VDVUeG5YY2p2S29mdFJpZnJXVXN1NlI1OGh5c0NHbTRwTDQ9?name="/>
-    <hyperlink ref="B10" r:id="rId18" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUnF2Qm1DaStXa3poWTNGZG5nak1qdTNkZzFSL096cVROOCtSazJwVFNkSTA9?name="/>
-    <hyperlink ref="B11" r:id="rId19" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUisxRTVjZElWekRWd245elFiQzVvbVAva1N4TWIwU0ZlUVFteTFkb29URlU9?name="/>
-    <hyperlink ref="B12" r:id="rId20" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUmc1OWw3djlOSlRXM2FOelMwSmxXZ0ZMcHJ6LzhOcHRTRzVLaEtxYjFkdVE9?name="/>
-    <hyperlink ref="B14" r:id="rId21" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUkh3NjZSWTBBT2xYWU45WElXd0RSM1kwR0g2ejhldzZodkpGZXVNVU1wTTQ9?name="/>
-    <hyperlink ref="C10" r:id="rId22" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUnF2Qm1DaStXa3poWTNGZG5nak1qdTROSVVuajdmQnJpMzlhSVo3TFI1cTA9?name="/>
-    <hyperlink ref="C12" r:id="rId23" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUmc1OWw3djlOSlRXM2FOelMwSmxXZ001STBRRG00bVo0d0UzaDY3ZUFGS1k9?name="/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -3269,8 +3098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" view="pageLayout" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -3284,15 +3113,15 @@
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -3316,57 +3145,57 @@
     <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
     </row>
     <row r="23" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="44"/>
+      <c r="C25" s="46"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="43" t="s">
+      <c r="E25" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="44"/>
+      <c r="F25" s="46"/>
     </row>
     <row r="26" spans="2:6" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="38"/>
-      <c r="E26" s="39" t="s">
+      <c r="C26" s="40"/>
+      <c r="E26" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="F26" s="40"/>
+      <c r="F26" s="42"/>
     </row>
     <row r="27" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="47"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="47"/>
+      <c r="C27" s="49"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="49"/>
     </row>
     <row r="28" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="37">
+      <c r="B28" s="39">
         <v>31200</v>
       </c>
-      <c r="C28" s="38"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="38"/>
+      <c r="C28" s="40"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="40"/>
     </row>
     <row r="29" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="49"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="49"/>
+      <c r="C29" s="51"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="51"/>
     </row>
     <row r="30" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3392,13 +3221,13 @@
     <row r="35" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="45" t="s">
+      <c r="B37" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
     </row>
     <row r="38" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3439,7 +3268,7 @@
   <dimension ref="A3:K354"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3457,15 +3286,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
     </row>
     <row r="6" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
@@ -3473,15 +3302,15 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
     </row>
     <row r="25" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
@@ -3492,37 +3321,37 @@
       <c r="A26" s="9"/>
     </row>
     <row r="27" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="52" t="s">
+      <c r="B27" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52" t="s">
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="52"/>
+      <c r="F27" s="54"/>
     </row>
     <row r="28" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="52" t="s">
+      <c r="B28" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52" t="s">
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="F28" s="52"/>
+      <c r="F28" s="54"/>
     </row>
     <row r="29" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="52" t="s">
+      <c r="B29" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52">
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54">
         <v>103</v>
       </c>
-      <c r="F29" s="52"/>
+      <c r="F29" s="54"/>
     </row>
     <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
@@ -3530,225 +3359,225 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="53" t="s">
+      <c r="A33" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
-      <c r="E33" s="53" t="s">
+      <c r="B33" s="55"/>
+      <c r="C33" s="55"/>
+      <c r="E33" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
     </row>
     <row r="34" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="78" t="s">
+      <c r="A34" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-      <c r="E34" s="78" t="s">
+      <c r="B34" s="72"/>
+      <c r="C34" s="72"/>
+      <c r="E34" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
+      <c r="F34" s="72"/>
+      <c r="G34" s="72"/>
     </row>
     <row r="35" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="72" t="s">
         <v>104</v>
       </c>
-      <c r="B35" s="78"/>
-      <c r="C35" s="78"/>
-      <c r="E35" s="78" t="s">
+      <c r="B35" s="72"/>
+      <c r="C35" s="72"/>
+      <c r="E35" s="72" t="s">
         <v>104</v>
       </c>
-      <c r="F35" s="78"/>
-      <c r="G35" s="78"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
     </row>
     <row r="36" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="78" t="s">
+      <c r="A36" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="B36" s="78"/>
-      <c r="C36" s="78"/>
-      <c r="E36" s="78" t="s">
+      <c r="B36" s="72"/>
+      <c r="C36" s="72"/>
+      <c r="E36" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="F36" s="78"/>
-      <c r="G36" s="78"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
     </row>
     <row r="37" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="78" t="s">
+      <c r="A37" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="B37" s="78"/>
-      <c r="C37" s="78"/>
-      <c r="E37" s="78" t="s">
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
+      <c r="E37" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="F37" s="78"/>
-      <c r="G37" s="78"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="72"/>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="75"/>
-      <c r="B38" s="76"/>
-      <c r="C38" s="76"/>
-      <c r="E38" s="75"/>
-      <c r="F38" s="76"/>
-      <c r="G38" s="76"/>
+      <c r="A38" s="56"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="56"/>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="76"/>
-      <c r="B39" s="76"/>
-      <c r="C39" s="76"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="76"/>
-      <c r="G39" s="76"/>
+      <c r="A39" s="56"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="76"/>
-      <c r="B40" s="76"/>
-      <c r="C40" s="76"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="76"/>
-      <c r="G40" s="76"/>
+      <c r="A40" s="56"/>
+      <c r="B40" s="56"/>
+      <c r="C40" s="56"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="56"/>
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="76"/>
-      <c r="B41" s="76"/>
-      <c r="C41" s="76"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
-      <c r="G41" s="76"/>
+      <c r="A41" s="56"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="56"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="56"/>
+      <c r="G41" s="56"/>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="76"/>
-      <c r="B42" s="76"/>
-      <c r="C42" s="76"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="76"/>
-      <c r="G42" s="76"/>
+      <c r="A42" s="56"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="56"/>
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="76"/>
-      <c r="B43" s="76"/>
-      <c r="C43" s="76"/>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76"/>
-      <c r="G43" s="76"/>
+      <c r="A43" s="56"/>
+      <c r="B43" s="56"/>
+      <c r="C43" s="56"/>
+      <c r="E43" s="56"/>
+      <c r="F43" s="56"/>
+      <c r="G43" s="56"/>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="76"/>
-      <c r="B44" s="76"/>
-      <c r="C44" s="76"/>
-      <c r="E44" s="76"/>
-      <c r="F44" s="76"/>
-      <c r="G44" s="76"/>
+      <c r="A44" s="56"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="56"/>
+      <c r="E44" s="56"/>
+      <c r="F44" s="56"/>
+      <c r="G44" s="56"/>
     </row>
     <row r="45" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="53" t="s">
+      <c r="A46" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="B46" s="53"/>
-      <c r="C46" s="53"/>
-      <c r="E46" s="53" t="s">
+      <c r="B46" s="55"/>
+      <c r="C46" s="55"/>
+      <c r="E46" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
+      <c r="F46" s="55"/>
+      <c r="G46" s="55"/>
     </row>
     <row r="47" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="78" t="s">
+      <c r="A47" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="B47" s="78"/>
-      <c r="C47" s="78"/>
-      <c r="E47" s="78" t="s">
+      <c r="B47" s="72"/>
+      <c r="C47" s="72"/>
+      <c r="E47" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="F47" s="78"/>
-      <c r="G47" s="78"/>
+      <c r="F47" s="72"/>
+      <c r="G47" s="72"/>
     </row>
     <row r="48" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="78" t="s">
+      <c r="A48" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="B48" s="78"/>
-      <c r="C48" s="78"/>
-      <c r="E48" s="78" t="s">
+      <c r="B48" s="72"/>
+      <c r="C48" s="72"/>
+      <c r="E48" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="F48" s="78"/>
-      <c r="G48" s="78"/>
+      <c r="F48" s="72"/>
+      <c r="G48" s="72"/>
     </row>
     <row r="49" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="78" t="s">
+      <c r="A49" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="B49" s="78"/>
-      <c r="C49" s="78"/>
-      <c r="E49" s="78" t="s">
+      <c r="B49" s="72"/>
+      <c r="C49" s="72"/>
+      <c r="E49" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="F49" s="78"/>
-      <c r="G49" s="78"/>
+      <c r="F49" s="72"/>
+      <c r="G49" s="72"/>
     </row>
     <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="75"/>
-      <c r="B50" s="76"/>
-      <c r="C50" s="76"/>
-      <c r="E50" s="75"/>
-      <c r="F50" s="76"/>
-      <c r="G50" s="76"/>
+      <c r="A50" s="56"/>
+      <c r="B50" s="56"/>
+      <c r="C50" s="56"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="56"/>
+      <c r="G50" s="56"/>
     </row>
     <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="76"/>
-      <c r="B51" s="76"/>
-      <c r="C51" s="76"/>
-      <c r="E51" s="76"/>
-      <c r="F51" s="76"/>
-      <c r="G51" s="76"/>
+      <c r="A51" s="56"/>
+      <c r="B51" s="56"/>
+      <c r="C51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
     </row>
     <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="76"/>
-      <c r="B52" s="76"/>
-      <c r="C52" s="76"/>
-      <c r="E52" s="76"/>
-      <c r="F52" s="76"/>
-      <c r="G52" s="76"/>
+      <c r="A52" s="56"/>
+      <c r="B52" s="56"/>
+      <c r="C52" s="56"/>
+      <c r="E52" s="56"/>
+      <c r="F52" s="56"/>
+      <c r="G52" s="56"/>
     </row>
     <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="76"/>
-      <c r="B53" s="76"/>
-      <c r="C53" s="76"/>
-      <c r="E53" s="76"/>
-      <c r="F53" s="76"/>
-      <c r="G53" s="76"/>
+      <c r="A53" s="56"/>
+      <c r="B53" s="56"/>
+      <c r="C53" s="56"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="56"/>
     </row>
     <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="76"/>
-      <c r="B54" s="76"/>
-      <c r="C54" s="76"/>
-      <c r="E54" s="76"/>
-      <c r="F54" s="76"/>
-      <c r="G54" s="76"/>
+      <c r="A54" s="56"/>
+      <c r="B54" s="56"/>
+      <c r="C54" s="56"/>
+      <c r="E54" s="56"/>
+      <c r="F54" s="56"/>
+      <c r="G54" s="56"/>
     </row>
     <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="76"/>
-      <c r="B55" s="76"/>
-      <c r="C55" s="76"/>
-      <c r="E55" s="76"/>
-      <c r="F55" s="76"/>
-      <c r="G55" s="76"/>
+      <c r="A55" s="56"/>
+      <c r="B55" s="56"/>
+      <c r="C55" s="56"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="56"/>
+      <c r="G55" s="56"/>
     </row>
     <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="76"/>
-      <c r="B56" s="76"/>
-      <c r="C56" s="76"/>
-      <c r="E56" s="76"/>
-      <c r="F56" s="76"/>
-      <c r="G56" s="76"/>
+      <c r="A56" s="56"/>
+      <c r="B56" s="56"/>
+      <c r="C56" s="56"/>
+      <c r="E56" s="56"/>
+      <c r="F56" s="56"/>
+      <c r="G56" s="56"/>
     </row>
     <row r="57" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3758,13 +3587,13 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="53" t="s">
+      <c r="B60" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="C60" s="53"/>
-      <c r="D60" s="53"/>
-      <c r="E60" s="53"/>
-      <c r="F60" s="53"/>
+      <c r="C60" s="55"/>
+      <c r="D60" s="55"/>
+      <c r="E60" s="55"/>
+      <c r="F60" s="55"/>
     </row>
     <row r="61" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="80" t="s">
@@ -3772,10 +3601,10 @@
       </c>
       <c r="C61" s="81"/>
       <c r="D61" s="82"/>
-      <c r="E61" s="61" t="s">
+      <c r="E61" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="F61" s="61"/>
+      <c r="F61" s="57"/>
     </row>
     <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="83" t="s">
@@ -3783,10 +3612,10 @@
       </c>
       <c r="C62" s="84"/>
       <c r="D62" s="85"/>
-      <c r="E62" s="61">
+      <c r="E62" s="57">
         <v>0.3</v>
       </c>
-      <c r="F62" s="61"/>
+      <c r="F62" s="57"/>
     </row>
     <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="80" t="s">
@@ -3794,10 +3623,10 @@
       </c>
       <c r="C63" s="81"/>
       <c r="D63" s="82"/>
-      <c r="E63" s="61" t="s">
+      <c r="E63" s="57" t="s">
         <v>117</v>
       </c>
-      <c r="F63" s="61"/>
+      <c r="F63" s="57"/>
     </row>
     <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="80" t="s">
@@ -3805,8 +3634,8 @@
       </c>
       <c r="C64" s="81"/>
       <c r="D64" s="82"/>
-      <c r="E64" s="61"/>
-      <c r="F64" s="61"/>
+      <c r="E64" s="57"/>
+      <c r="F64" s="57"/>
     </row>
     <row r="65" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="80" t="s">
@@ -3814,8 +3643,8 @@
       </c>
       <c r="C65" s="81"/>
       <c r="D65" s="82"/>
-      <c r="E65" s="61"/>
-      <c r="F65" s="61"/>
+      <c r="E65" s="57"/>
+      <c r="F65" s="57"/>
     </row>
     <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="80" t="s">
@@ -3823,119 +3652,119 @@
       </c>
       <c r="C66" s="81"/>
       <c r="D66" s="82"/>
-      <c r="E66" s="61"/>
-      <c r="F66" s="61"/>
+      <c r="E66" s="57"/>
+      <c r="F66" s="57"/>
     </row>
     <row r="67" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="75"/>
-      <c r="C67" s="76"/>
-      <c r="D67" s="76"/>
-      <c r="E67" s="76"/>
-      <c r="F67" s="76"/>
+      <c r="B67" s="56"/>
+      <c r="C67" s="56"/>
+      <c r="D67" s="56"/>
+      <c r="E67" s="56"/>
+      <c r="F67" s="56"/>
     </row>
     <row r="68" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="76"/>
-      <c r="C68" s="76"/>
-      <c r="D68" s="76"/>
-      <c r="E68" s="76"/>
-      <c r="F68" s="76"/>
+      <c r="B68" s="56"/>
+      <c r="C68" s="56"/>
+      <c r="D68" s="56"/>
+      <c r="E68" s="56"/>
+      <c r="F68" s="56"/>
     </row>
     <row r="69" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="76"/>
-      <c r="C69" s="76"/>
-      <c r="D69" s="76"/>
-      <c r="E69" s="76"/>
-      <c r="F69" s="76"/>
+      <c r="B69" s="56"/>
+      <c r="C69" s="56"/>
+      <c r="D69" s="56"/>
+      <c r="E69" s="56"/>
+      <c r="F69" s="56"/>
     </row>
     <row r="70" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="76"/>
-      <c r="C70" s="76"/>
-      <c r="D70" s="76"/>
-      <c r="E70" s="76"/>
-      <c r="F70" s="76"/>
+      <c r="B70" s="56"/>
+      <c r="C70" s="56"/>
+      <c r="D70" s="56"/>
+      <c r="E70" s="56"/>
+      <c r="F70" s="56"/>
     </row>
     <row r="71" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="76"/>
-      <c r="C71" s="76"/>
-      <c r="D71" s="76"/>
-      <c r="E71" s="76"/>
-      <c r="F71" s="76"/>
+      <c r="B71" s="56"/>
+      <c r="C71" s="56"/>
+      <c r="D71" s="56"/>
+      <c r="E71" s="56"/>
+      <c r="F71" s="56"/>
     </row>
     <row r="72" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="76"/>
-      <c r="C72" s="76"/>
-      <c r="D72" s="76"/>
-      <c r="E72" s="76"/>
-      <c r="F72" s="76"/>
+      <c r="B72" s="56"/>
+      <c r="C72" s="56"/>
+      <c r="D72" s="56"/>
+      <c r="E72" s="56"/>
+      <c r="F72" s="56"/>
     </row>
     <row r="73" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="76"/>
-      <c r="C73" s="76"/>
-      <c r="D73" s="76"/>
-      <c r="E73" s="76"/>
-      <c r="F73" s="76"/>
+      <c r="B73" s="56"/>
+      <c r="C73" s="56"/>
+      <c r="D73" s="56"/>
+      <c r="E73" s="56"/>
+      <c r="F73" s="56"/>
     </row>
     <row r="74" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="76" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="53" t="s">
+      <c r="B76" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="C76" s="53"/>
-      <c r="D76" s="53"/>
-      <c r="E76" s="53"/>
-      <c r="F76" s="53"/>
+      <c r="C76" s="55"/>
+      <c r="D76" s="55"/>
+      <c r="E76" s="55"/>
+      <c r="F76" s="55"/>
     </row>
     <row r="77" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="77" t="s">
+      <c r="B77" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="C77" s="77"/>
-      <c r="D77" s="77"/>
-      <c r="E77" s="61" t="s">
+      <c r="C77" s="66"/>
+      <c r="D77" s="66"/>
+      <c r="E77" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="F77" s="61"/>
+      <c r="F77" s="57"/>
     </row>
     <row r="78" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="77" t="s">
+      <c r="B78" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="C78" s="77"/>
-      <c r="D78" s="77"/>
-      <c r="E78" s="61">
+      <c r="C78" s="66"/>
+      <c r="D78" s="66"/>
+      <c r="E78" s="57">
         <v>0.3</v>
       </c>
-      <c r="F78" s="61"/>
+      <c r="F78" s="57"/>
     </row>
     <row r="79" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="77" t="s">
+      <c r="B79" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="C79" s="77"/>
-      <c r="D79" s="77"/>
-      <c r="E79" s="61" t="s">
+      <c r="C79" s="66"/>
+      <c r="D79" s="66"/>
+      <c r="E79" s="57" t="s">
         <v>117</v>
       </c>
-      <c r="F79" s="61"/>
+      <c r="F79" s="57"/>
     </row>
     <row r="80" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="77" t="s">
+      <c r="B80" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="C80" s="77"/>
-      <c r="D80" s="77"/>
-      <c r="E80" s="61"/>
-      <c r="F80" s="61"/>
+      <c r="C80" s="66"/>
+      <c r="D80" s="66"/>
+      <c r="E80" s="57"/>
+      <c r="F80" s="57"/>
     </row>
     <row r="81" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="77" t="s">
+      <c r="B81" s="66" t="s">
         <v>119</v>
       </c>
-      <c r="C81" s="77"/>
-      <c r="D81" s="77"/>
-      <c r="E81" s="61"/>
-      <c r="F81" s="61"/>
+      <c r="C81" s="66"/>
+      <c r="D81" s="66"/>
+      <c r="E81" s="57"/>
+      <c r="F81" s="57"/>
     </row>
     <row r="82" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="80" t="s">
@@ -3943,129 +3772,129 @@
       </c>
       <c r="C82" s="81"/>
       <c r="D82" s="82"/>
-      <c r="E82" s="61"/>
-      <c r="F82" s="61"/>
+      <c r="E82" s="57"/>
+      <c r="F82" s="57"/>
     </row>
     <row r="83" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="75"/>
-      <c r="C83" s="76"/>
-      <c r="D83" s="76"/>
-      <c r="E83" s="76"/>
-      <c r="F83" s="76"/>
+      <c r="B83" s="56"/>
+      <c r="C83" s="56"/>
+      <c r="D83" s="56"/>
+      <c r="E83" s="56"/>
+      <c r="F83" s="56"/>
     </row>
     <row r="84" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="76"/>
-      <c r="C84" s="76"/>
-      <c r="D84" s="76"/>
-      <c r="E84" s="76"/>
-      <c r="F84" s="76"/>
+      <c r="B84" s="56"/>
+      <c r="C84" s="56"/>
+      <c r="D84" s="56"/>
+      <c r="E84" s="56"/>
+      <c r="F84" s="56"/>
     </row>
     <row r="85" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="76"/>
-      <c r="C85" s="76"/>
-      <c r="D85" s="76"/>
-      <c r="E85" s="76"/>
-      <c r="F85" s="76"/>
+      <c r="B85" s="56"/>
+      <c r="C85" s="56"/>
+      <c r="D85" s="56"/>
+      <c r="E85" s="56"/>
+      <c r="F85" s="56"/>
     </row>
     <row r="86" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="76"/>
-      <c r="C86" s="76"/>
-      <c r="D86" s="76"/>
-      <c r="E86" s="76"/>
-      <c r="F86" s="76"/>
+      <c r="B86" s="56"/>
+      <c r="C86" s="56"/>
+      <c r="D86" s="56"/>
+      <c r="E86" s="56"/>
+      <c r="F86" s="56"/>
     </row>
     <row r="87" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="76"/>
-      <c r="C87" s="76"/>
-      <c r="D87" s="76"/>
-      <c r="E87" s="76"/>
-      <c r="F87" s="76"/>
+      <c r="B87" s="56"/>
+      <c r="C87" s="56"/>
+      <c r="D87" s="56"/>
+      <c r="E87" s="56"/>
+      <c r="F87" s="56"/>
     </row>
     <row r="88" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="76"/>
-      <c r="C88" s="76"/>
-      <c r="D88" s="76"/>
-      <c r="E88" s="76"/>
-      <c r="F88" s="76"/>
+      <c r="B88" s="56"/>
+      <c r="C88" s="56"/>
+      <c r="D88" s="56"/>
+      <c r="E88" s="56"/>
+      <c r="F88" s="56"/>
     </row>
     <row r="89" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="76"/>
-      <c r="C89" s="76"/>
-      <c r="D89" s="76"/>
-      <c r="E89" s="76"/>
-      <c r="F89" s="76"/>
+      <c r="B89" s="56"/>
+      <c r="C89" s="56"/>
+      <c r="D89" s="56"/>
+      <c r="E89" s="56"/>
+      <c r="F89" s="56"/>
     </row>
     <row r="90" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="91" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="53" t="s">
+      <c r="B91" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="C91" s="53"/>
-      <c r="D91" s="53"/>
-      <c r="E91" s="53"/>
-      <c r="F91" s="53"/>
+      <c r="C91" s="55"/>
+      <c r="D91" s="55"/>
+      <c r="E91" s="55"/>
+      <c r="F91" s="55"/>
     </row>
     <row r="92" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="77" t="s">
+      <c r="B92" s="66" t="s">
         <v>123</v>
       </c>
-      <c r="C92" s="77"/>
-      <c r="D92" s="77"/>
-      <c r="E92" s="64" t="s">
+      <c r="C92" s="66"/>
+      <c r="D92" s="66"/>
+      <c r="E92" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="F92" s="65"/>
+      <c r="F92" s="61"/>
     </row>
     <row r="93" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="77" t="s">
+      <c r="B93" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="C93" s="77"/>
-      <c r="D93" s="77"/>
-      <c r="E93" s="66" t="s">
+      <c r="C93" s="66"/>
+      <c r="D93" s="66"/>
+      <c r="E93" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="F93" s="67"/>
+      <c r="F93" s="63"/>
     </row>
     <row r="94" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="77" t="s">
+      <c r="B94" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="C94" s="77"/>
-      <c r="D94" s="77"/>
-      <c r="E94" s="66" t="s">
+      <c r="C94" s="66"/>
+      <c r="D94" s="66"/>
+      <c r="E94" s="62" t="s">
         <v>117</v>
       </c>
-      <c r="F94" s="67"/>
+      <c r="F94" s="63"/>
     </row>
     <row r="95" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="77" t="s">
+      <c r="B95" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="C95" s="77"/>
-      <c r="D95" s="77"/>
-      <c r="E95" s="66"/>
-      <c r="F95" s="67"/>
+      <c r="C95" s="66"/>
+      <c r="D95" s="66"/>
+      <c r="E95" s="62"/>
+      <c r="F95" s="63"/>
     </row>
     <row r="96" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="77" t="s">
+      <c r="B96" s="66" t="s">
         <v>119</v>
       </c>
-      <c r="C96" s="77"/>
-      <c r="D96" s="77"/>
-      <c r="E96" s="62"/>
-      <c r="F96" s="63"/>
+      <c r="C96" s="66"/>
+      <c r="D96" s="66"/>
+      <c r="E96" s="58"/>
+      <c r="F96" s="59"/>
     </row>
     <row r="97" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="77" t="s">
+      <c r="B97" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="C97" s="77"/>
-      <c r="D97" s="77"/>
-      <c r="E97" s="62">
+      <c r="C97" s="66"/>
+      <c r="D97" s="66"/>
+      <c r="E97" s="58">
         <v>62</v>
       </c>
-      <c r="F97" s="63"/>
+      <c r="F97" s="59"/>
     </row>
     <row r="98" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="80" t="s">
@@ -4073,129 +3902,129 @@
       </c>
       <c r="C98" s="81"/>
       <c r="D98" s="82"/>
-      <c r="E98" s="61"/>
-      <c r="F98" s="61"/>
+      <c r="E98" s="57"/>
+      <c r="F98" s="57"/>
     </row>
     <row r="99" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="75"/>
-      <c r="C99" s="76"/>
-      <c r="D99" s="76"/>
-      <c r="E99" s="76"/>
-      <c r="F99" s="76"/>
+      <c r="B99" s="56"/>
+      <c r="C99" s="56"/>
+      <c r="D99" s="56"/>
+      <c r="E99" s="56"/>
+      <c r="F99" s="56"/>
     </row>
     <row r="100" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="76"/>
-      <c r="C100" s="76"/>
-      <c r="D100" s="76"/>
-      <c r="E100" s="76"/>
-      <c r="F100" s="76"/>
+      <c r="B100" s="56"/>
+      <c r="C100" s="56"/>
+      <c r="D100" s="56"/>
+      <c r="E100" s="56"/>
+      <c r="F100" s="56"/>
     </row>
     <row r="101" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="76"/>
-      <c r="C101" s="76"/>
-      <c r="D101" s="76"/>
-      <c r="E101" s="76"/>
-      <c r="F101" s="76"/>
+      <c r="B101" s="56"/>
+      <c r="C101" s="56"/>
+      <c r="D101" s="56"/>
+      <c r="E101" s="56"/>
+      <c r="F101" s="56"/>
     </row>
     <row r="102" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="76"/>
-      <c r="C102" s="76"/>
-      <c r="D102" s="76"/>
-      <c r="E102" s="76"/>
-      <c r="F102" s="76"/>
+      <c r="B102" s="56"/>
+      <c r="C102" s="56"/>
+      <c r="D102" s="56"/>
+      <c r="E102" s="56"/>
+      <c r="F102" s="56"/>
     </row>
     <row r="103" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="76"/>
-      <c r="C103" s="76"/>
-      <c r="D103" s="76"/>
-      <c r="E103" s="76"/>
-      <c r="F103" s="76"/>
+      <c r="B103" s="56"/>
+      <c r="C103" s="56"/>
+      <c r="D103" s="56"/>
+      <c r="E103" s="56"/>
+      <c r="F103" s="56"/>
     </row>
     <row r="104" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="76"/>
-      <c r="C104" s="76"/>
-      <c r="D104" s="76"/>
-      <c r="E104" s="76"/>
-      <c r="F104" s="76"/>
+      <c r="B104" s="56"/>
+      <c r="C104" s="56"/>
+      <c r="D104" s="56"/>
+      <c r="E104" s="56"/>
+      <c r="F104" s="56"/>
     </row>
     <row r="105" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="76"/>
-      <c r="C105" s="76"/>
-      <c r="D105" s="76"/>
-      <c r="E105" s="76"/>
-      <c r="F105" s="76"/>
+      <c r="B105" s="56"/>
+      <c r="C105" s="56"/>
+      <c r="D105" s="56"/>
+      <c r="E105" s="56"/>
+      <c r="F105" s="56"/>
     </row>
     <row r="106" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="107" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="53" t="s">
+      <c r="B107" s="55" t="s">
         <v>127</v>
       </c>
-      <c r="C107" s="53"/>
-      <c r="D107" s="53"/>
-      <c r="E107" s="53"/>
-      <c r="F107" s="53"/>
+      <c r="C107" s="55"/>
+      <c r="D107" s="55"/>
+      <c r="E107" s="55"/>
+      <c r="F107" s="55"/>
     </row>
     <row r="108" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="77" t="s">
+      <c r="B108" s="66" t="s">
         <v>123</v>
       </c>
-      <c r="C108" s="77"/>
-      <c r="D108" s="77"/>
-      <c r="E108" s="64" t="s">
+      <c r="C108" s="66"/>
+      <c r="D108" s="66"/>
+      <c r="E108" s="60" t="s">
         <v>128</v>
       </c>
-      <c r="F108" s="65"/>
+      <c r="F108" s="61"/>
     </row>
     <row r="109" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="77" t="s">
+      <c r="B109" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="C109" s="77"/>
-      <c r="D109" s="77"/>
-      <c r="E109" s="66" t="s">
+      <c r="C109" s="66"/>
+      <c r="D109" s="66"/>
+      <c r="E109" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="F109" s="67"/>
+      <c r="F109" s="63"/>
     </row>
     <row r="110" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="77" t="s">
+      <c r="B110" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="C110" s="77"/>
-      <c r="D110" s="77"/>
-      <c r="E110" s="66" t="s">
+      <c r="C110" s="66"/>
+      <c r="D110" s="66"/>
+      <c r="E110" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="F110" s="67"/>
+      <c r="F110" s="63"/>
     </row>
     <row r="111" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="77" t="s">
+      <c r="B111" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="C111" s="77"/>
-      <c r="D111" s="77"/>
-      <c r="E111" s="66"/>
-      <c r="F111" s="67"/>
+      <c r="C111" s="66"/>
+      <c r="D111" s="66"/>
+      <c r="E111" s="62"/>
+      <c r="F111" s="63"/>
     </row>
     <row r="112" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="77" t="s">
+      <c r="B112" s="66" t="s">
         <v>119</v>
       </c>
-      <c r="C112" s="77"/>
-      <c r="D112" s="77"/>
-      <c r="E112" s="62" t="s">
+      <c r="C112" s="66"/>
+      <c r="D112" s="66"/>
+      <c r="E112" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="F112" s="63"/>
+      <c r="F112" s="59"/>
     </row>
     <row r="113" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="77" t="s">
+      <c r="B113" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="C113" s="77"/>
-      <c r="D113" s="77"/>
-      <c r="E113" s="62"/>
-      <c r="F113" s="63"/>
+      <c r="C113" s="66"/>
+      <c r="D113" s="66"/>
+      <c r="E113" s="58"/>
+      <c r="F113" s="59"/>
     </row>
     <row r="114" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B114" s="80" t="s">
@@ -4203,132 +4032,132 @@
       </c>
       <c r="C114" s="81"/>
       <c r="D114" s="82"/>
-      <c r="E114" s="61"/>
-      <c r="F114" s="61"/>
+      <c r="E114" s="57"/>
+      <c r="F114" s="57"/>
     </row>
     <row r="115" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="76"/>
-      <c r="C115" s="76"/>
-      <c r="D115" s="76"/>
-      <c r="E115" s="76"/>
-      <c r="F115" s="76"/>
+      <c r="B115" s="86"/>
+      <c r="C115" s="86"/>
+      <c r="D115" s="86"/>
+      <c r="E115" s="86"/>
+      <c r="F115" s="86"/>
     </row>
     <row r="116" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="76"/>
-      <c r="C116" s="76"/>
-      <c r="D116" s="76"/>
-      <c r="E116" s="76"/>
-      <c r="F116" s="76"/>
+      <c r="B116" s="86"/>
+      <c r="C116" s="86"/>
+      <c r="D116" s="86"/>
+      <c r="E116" s="86"/>
+      <c r="F116" s="86"/>
     </row>
     <row r="117" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="76"/>
-      <c r="C117" s="76"/>
-      <c r="D117" s="76"/>
-      <c r="E117" s="76"/>
-      <c r="F117" s="76"/>
+      <c r="B117" s="86"/>
+      <c r="C117" s="86"/>
+      <c r="D117" s="86"/>
+      <c r="E117" s="86"/>
+      <c r="F117" s="86"/>
     </row>
     <row r="118" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="76"/>
-      <c r="C118" s="76"/>
-      <c r="D118" s="76"/>
-      <c r="E118" s="76"/>
-      <c r="F118" s="76"/>
+      <c r="B118" s="86"/>
+      <c r="C118" s="86"/>
+      <c r="D118" s="86"/>
+      <c r="E118" s="86"/>
+      <c r="F118" s="86"/>
     </row>
     <row r="119" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="76"/>
-      <c r="C119" s="76"/>
-      <c r="D119" s="76"/>
-      <c r="E119" s="76"/>
-      <c r="F119" s="76"/>
+      <c r="B119" s="86"/>
+      <c r="C119" s="86"/>
+      <c r="D119" s="86"/>
+      <c r="E119" s="86"/>
+      <c r="F119" s="86"/>
     </row>
     <row r="120" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="76"/>
-      <c r="C120" s="76"/>
-      <c r="D120" s="76"/>
-      <c r="E120" s="76"/>
-      <c r="F120" s="76"/>
+      <c r="B120" s="86"/>
+      <c r="C120" s="86"/>
+      <c r="D120" s="86"/>
+      <c r="E120" s="86"/>
+      <c r="F120" s="86"/>
     </row>
     <row r="121" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="76"/>
-      <c r="C121" s="76"/>
-      <c r="D121" s="76"/>
-      <c r="E121" s="76"/>
-      <c r="F121" s="76"/>
+      <c r="B121" s="86"/>
+      <c r="C121" s="86"/>
+      <c r="D121" s="86"/>
+      <c r="E121" s="86"/>
+      <c r="F121" s="86"/>
     </row>
     <row r="123" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="53" t="s">
+      <c r="B123" s="55" t="s">
         <v>129</v>
       </c>
-      <c r="C123" s="53"/>
-      <c r="D123" s="53"/>
-      <c r="E123" s="53"/>
-      <c r="F123" s="53"/>
+      <c r="C123" s="55"/>
+      <c r="D123" s="55"/>
+      <c r="E123" s="55"/>
+      <c r="F123" s="55"/>
     </row>
     <row r="124" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="77" t="s">
+      <c r="B124" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="C124" s="77"/>
-      <c r="D124" s="77"/>
-      <c r="E124" s="64" t="s">
+      <c r="C124" s="66"/>
+      <c r="D124" s="66"/>
+      <c r="E124" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="F124" s="65"/>
+      <c r="F124" s="61"/>
     </row>
     <row r="125" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="77" t="s">
+      <c r="B125" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="C125" s="77"/>
-      <c r="D125" s="77"/>
-      <c r="E125" s="66" t="s">
+      <c r="C125" s="66"/>
+      <c r="D125" s="66"/>
+      <c r="E125" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="F125" s="67"/>
+      <c r="F125" s="63"/>
     </row>
     <row r="126" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="77" t="s">
+      <c r="B126" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="C126" s="77"/>
-      <c r="D126" s="77"/>
-      <c r="E126" s="66" t="s">
+      <c r="C126" s="66"/>
+      <c r="D126" s="66"/>
+      <c r="E126" s="62" t="s">
         <v>132</v>
       </c>
-      <c r="F126" s="67"/>
+      <c r="F126" s="63"/>
     </row>
     <row r="127" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="77" t="s">
+      <c r="B127" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="C127" s="77"/>
-      <c r="D127" s="77"/>
-      <c r="E127" s="66">
+      <c r="C127" s="66"/>
+      <c r="D127" s="66"/>
+      <c r="E127" s="62">
         <v>0.06</v>
       </c>
-      <c r="F127" s="67"/>
+      <c r="F127" s="63"/>
     </row>
     <row r="128" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="77" t="s">
+      <c r="B128" s="66" t="s">
         <v>119</v>
       </c>
-      <c r="C128" s="77"/>
-      <c r="D128" s="77"/>
-      <c r="E128" s="62" t="s">
+      <c r="C128" s="66"/>
+      <c r="D128" s="66"/>
+      <c r="E128" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="F128" s="63"/>
+      <c r="F128" s="59"/>
     </row>
     <row r="129" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="77" t="s">
+      <c r="B129" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="C129" s="77"/>
-      <c r="D129" s="77"/>
-      <c r="E129" s="62">
+      <c r="C129" s="66"/>
+      <c r="D129" s="66"/>
+      <c r="E129" s="58">
         <v>48.75</v>
       </c>
-      <c r="F129" s="63"/>
+      <c r="F129" s="59"/>
     </row>
     <row r="130" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B130" s="80" t="s">
@@ -4336,128 +4165,128 @@
       </c>
       <c r="C130" s="81"/>
       <c r="D130" s="82"/>
-      <c r="E130" s="61"/>
-      <c r="F130" s="61"/>
+      <c r="E130" s="57"/>
+      <c r="F130" s="57"/>
     </row>
     <row r="131" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="75"/>
-      <c r="C131" s="76"/>
-      <c r="D131" s="76"/>
-      <c r="E131" s="76"/>
-      <c r="F131" s="76"/>
+      <c r="B131" s="56"/>
+      <c r="C131" s="56"/>
+      <c r="D131" s="56"/>
+      <c r="E131" s="56"/>
+      <c r="F131" s="56"/>
     </row>
     <row r="132" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="76"/>
-      <c r="C132" s="76"/>
-      <c r="D132" s="76"/>
-      <c r="E132" s="76"/>
-      <c r="F132" s="76"/>
+      <c r="B132" s="56"/>
+      <c r="C132" s="56"/>
+      <c r="D132" s="56"/>
+      <c r="E132" s="56"/>
+      <c r="F132" s="56"/>
     </row>
     <row r="133" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="76"/>
-      <c r="C133" s="76"/>
-      <c r="D133" s="76"/>
-      <c r="E133" s="76"/>
-      <c r="F133" s="76"/>
+      <c r="B133" s="56"/>
+      <c r="C133" s="56"/>
+      <c r="D133" s="56"/>
+      <c r="E133" s="56"/>
+      <c r="F133" s="56"/>
     </row>
     <row r="134" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="76"/>
-      <c r="C134" s="76"/>
-      <c r="D134" s="76"/>
-      <c r="E134" s="76"/>
-      <c r="F134" s="76"/>
+      <c r="B134" s="56"/>
+      <c r="C134" s="56"/>
+      <c r="D134" s="56"/>
+      <c r="E134" s="56"/>
+      <c r="F134" s="56"/>
     </row>
     <row r="135" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="76"/>
-      <c r="C135" s="76"/>
-      <c r="D135" s="76"/>
-      <c r="E135" s="76"/>
-      <c r="F135" s="76"/>
+      <c r="B135" s="56"/>
+      <c r="C135" s="56"/>
+      <c r="D135" s="56"/>
+      <c r="E135" s="56"/>
+      <c r="F135" s="56"/>
     </row>
     <row r="136" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="76"/>
-      <c r="C136" s="76"/>
-      <c r="D136" s="76"/>
-      <c r="E136" s="76"/>
-      <c r="F136" s="76"/>
+      <c r="B136" s="56"/>
+      <c r="C136" s="56"/>
+      <c r="D136" s="56"/>
+      <c r="E136" s="56"/>
+      <c r="F136" s="56"/>
     </row>
     <row r="137" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="76"/>
-      <c r="C137" s="76"/>
-      <c r="D137" s="76"/>
-      <c r="E137" s="76"/>
-      <c r="F137" s="76"/>
+      <c r="B137" s="56"/>
+      <c r="C137" s="56"/>
+      <c r="D137" s="56"/>
+      <c r="E137" s="56"/>
+      <c r="F137" s="56"/>
     </row>
     <row r="139" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="53" t="s">
+      <c r="B139" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="C139" s="53"/>
-      <c r="D139" s="53"/>
-      <c r="E139" s="53"/>
-      <c r="F139" s="53"/>
+      <c r="C139" s="55"/>
+      <c r="D139" s="55"/>
+      <c r="E139" s="55"/>
+      <c r="F139" s="55"/>
     </row>
     <row r="140" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="77" t="s">
+      <c r="B140" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="C140" s="77"/>
-      <c r="D140" s="77"/>
-      <c r="E140" s="64" t="s">
+      <c r="C140" s="66"/>
+      <c r="D140" s="66"/>
+      <c r="E140" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="F140" s="65"/>
+      <c r="F140" s="61"/>
     </row>
     <row r="141" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="77" t="s">
+      <c r="B141" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="C141" s="77"/>
-      <c r="D141" s="77"/>
-      <c r="E141" s="66" t="s">
+      <c r="C141" s="66"/>
+      <c r="D141" s="66"/>
+      <c r="E141" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="F141" s="67"/>
+      <c r="F141" s="63"/>
     </row>
     <row r="142" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="77" t="s">
+      <c r="B142" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="C142" s="77"/>
-      <c r="D142" s="77"/>
-      <c r="E142" s="66" t="s">
+      <c r="C142" s="66"/>
+      <c r="D142" s="66"/>
+      <c r="E142" s="62" t="s">
         <v>117</v>
       </c>
-      <c r="F142" s="67"/>
+      <c r="F142" s="63"/>
     </row>
     <row r="143" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="77" t="s">
+      <c r="B143" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="C143" s="77"/>
-      <c r="D143" s="77"/>
-      <c r="E143" s="66"/>
-      <c r="F143" s="67"/>
+      <c r="C143" s="66"/>
+      <c r="D143" s="66"/>
+      <c r="E143" s="62"/>
+      <c r="F143" s="63"/>
     </row>
     <row r="144" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="77" t="s">
+      <c r="B144" s="66" t="s">
         <v>119</v>
       </c>
-      <c r="C144" s="77"/>
-      <c r="D144" s="77"/>
-      <c r="E144" s="62"/>
-      <c r="F144" s="63"/>
+      <c r="C144" s="66"/>
+      <c r="D144" s="66"/>
+      <c r="E144" s="58"/>
+      <c r="F144" s="59"/>
     </row>
     <row r="145" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="77" t="s">
+      <c r="B145" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="C145" s="77"/>
-      <c r="D145" s="77"/>
-      <c r="E145" s="62">
+      <c r="C145" s="66"/>
+      <c r="D145" s="66"/>
+      <c r="E145" s="58">
         <v>13.25</v>
       </c>
-      <c r="F145" s="63"/>
+      <c r="F145" s="59"/>
     </row>
     <row r="146" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B146" s="80" t="s">
@@ -4465,445 +4294,445 @@
       </c>
       <c r="C146" s="81"/>
       <c r="D146" s="82"/>
-      <c r="E146" s="61"/>
-      <c r="F146" s="61"/>
+      <c r="E146" s="57"/>
+      <c r="F146" s="57"/>
     </row>
     <row r="147" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="75"/>
-      <c r="C147" s="76"/>
-      <c r="D147" s="76"/>
-      <c r="E147" s="76"/>
-      <c r="F147" s="76"/>
+      <c r="B147" s="56"/>
+      <c r="C147" s="56"/>
+      <c r="D147" s="56"/>
+      <c r="E147" s="56"/>
+      <c r="F147" s="56"/>
     </row>
     <row r="148" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="76"/>
-      <c r="C148" s="76"/>
-      <c r="D148" s="76"/>
-      <c r="E148" s="76"/>
-      <c r="F148" s="76"/>
+      <c r="B148" s="56"/>
+      <c r="C148" s="56"/>
+      <c r="D148" s="56"/>
+      <c r="E148" s="56"/>
+      <c r="F148" s="56"/>
     </row>
     <row r="149" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="76"/>
-      <c r="C149" s="76"/>
-      <c r="D149" s="76"/>
-      <c r="E149" s="76"/>
-      <c r="F149" s="76"/>
+      <c r="B149" s="56"/>
+      <c r="C149" s="56"/>
+      <c r="D149" s="56"/>
+      <c r="E149" s="56"/>
+      <c r="F149" s="56"/>
     </row>
     <row r="150" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="76"/>
-      <c r="C150" s="76"/>
-      <c r="D150" s="76"/>
-      <c r="E150" s="76"/>
-      <c r="F150" s="76"/>
+      <c r="B150" s="56"/>
+      <c r="C150" s="56"/>
+      <c r="D150" s="56"/>
+      <c r="E150" s="56"/>
+      <c r="F150" s="56"/>
     </row>
     <row r="151" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="76"/>
-      <c r="C151" s="76"/>
-      <c r="D151" s="76"/>
-      <c r="E151" s="76"/>
-      <c r="F151" s="76"/>
+      <c r="B151" s="56"/>
+      <c r="C151" s="56"/>
+      <c r="D151" s="56"/>
+      <c r="E151" s="56"/>
+      <c r="F151" s="56"/>
     </row>
     <row r="152" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="76"/>
-      <c r="C152" s="76"/>
-      <c r="D152" s="76"/>
-      <c r="E152" s="76"/>
-      <c r="F152" s="76"/>
+      <c r="B152" s="56"/>
+      <c r="C152" s="56"/>
+      <c r="D152" s="56"/>
+      <c r="E152" s="56"/>
+      <c r="F152" s="56"/>
     </row>
     <row r="153" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="76"/>
-      <c r="C153" s="76"/>
-      <c r="D153" s="76"/>
-      <c r="E153" s="76"/>
-      <c r="F153" s="76"/>
+      <c r="B153" s="56"/>
+      <c r="C153" s="56"/>
+      <c r="D153" s="56"/>
+      <c r="E153" s="56"/>
+      <c r="F153" s="56"/>
     </row>
     <row r="155" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="53" t="s">
+      <c r="B155" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="C155" s="53"/>
-      <c r="D155" s="53"/>
-      <c r="E155" s="53"/>
-      <c r="F155" s="53"/>
+      <c r="C155" s="55"/>
+      <c r="D155" s="55"/>
+      <c r="E155" s="55"/>
+      <c r="F155" s="55"/>
     </row>
     <row r="156" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="77" t="s">
+      <c r="B156" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="C156" s="77"/>
-      <c r="D156" s="77"/>
-      <c r="E156" s="64" t="s">
+      <c r="C156" s="66"/>
+      <c r="D156" s="66"/>
+      <c r="E156" s="60" t="s">
         <v>136</v>
       </c>
-      <c r="F156" s="65"/>
+      <c r="F156" s="61"/>
     </row>
     <row r="157" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B157" s="77" t="s">
+      <c r="B157" s="66" t="s">
         <v>137</v>
       </c>
-      <c r="C157" s="77"/>
-      <c r="D157" s="77"/>
-      <c r="E157" s="66" t="s">
+      <c r="C157" s="66"/>
+      <c r="D157" s="66"/>
+      <c r="E157" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="F157" s="67"/>
+      <c r="F157" s="63"/>
     </row>
     <row r="158" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="77" t="s">
+      <c r="B158" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="C158" s="77"/>
-      <c r="D158" s="77"/>
-      <c r="E158" s="66" t="s">
+      <c r="C158" s="66"/>
+      <c r="D158" s="66"/>
+      <c r="E158" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="F158" s="67"/>
+      <c r="F158" s="63"/>
     </row>
     <row r="159" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="77" t="s">
+      <c r="B159" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="C159" s="77"/>
-      <c r="D159" s="77"/>
-      <c r="E159" s="62">
+      <c r="C159" s="66"/>
+      <c r="D159" s="66"/>
+      <c r="E159" s="58">
         <v>6</v>
       </c>
-      <c r="F159" s="63"/>
+      <c r="F159" s="59"/>
     </row>
     <row r="160" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="75"/>
-      <c r="C160" s="76"/>
-      <c r="D160" s="76"/>
-      <c r="E160" s="76"/>
-      <c r="F160" s="76"/>
+      <c r="B160" s="56"/>
+      <c r="C160" s="56"/>
+      <c r="D160" s="56"/>
+      <c r="E160" s="56"/>
+      <c r="F160" s="56"/>
     </row>
     <row r="161" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="76"/>
-      <c r="C161" s="76"/>
-      <c r="D161" s="76"/>
-      <c r="E161" s="76"/>
-      <c r="F161" s="76"/>
+      <c r="B161" s="56"/>
+      <c r="C161" s="56"/>
+      <c r="D161" s="56"/>
+      <c r="E161" s="56"/>
+      <c r="F161" s="56"/>
     </row>
     <row r="162" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="76"/>
-      <c r="C162" s="76"/>
-      <c r="D162" s="76"/>
-      <c r="E162" s="76"/>
-      <c r="F162" s="76"/>
+      <c r="B162" s="56"/>
+      <c r="C162" s="56"/>
+      <c r="D162" s="56"/>
+      <c r="E162" s="56"/>
+      <c r="F162" s="56"/>
     </row>
     <row r="163" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="76"/>
-      <c r="C163" s="76"/>
-      <c r="D163" s="76"/>
-      <c r="E163" s="76"/>
-      <c r="F163" s="76"/>
+      <c r="B163" s="56"/>
+      <c r="C163" s="56"/>
+      <c r="D163" s="56"/>
+      <c r="E163" s="56"/>
+      <c r="F163" s="56"/>
     </row>
     <row r="164" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="76"/>
-      <c r="C164" s="76"/>
-      <c r="D164" s="76"/>
-      <c r="E164" s="76"/>
-      <c r="F164" s="76"/>
+      <c r="B164" s="56"/>
+      <c r="C164" s="56"/>
+      <c r="D164" s="56"/>
+      <c r="E164" s="56"/>
+      <c r="F164" s="56"/>
     </row>
     <row r="165" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="76"/>
-      <c r="C165" s="76"/>
-      <c r="D165" s="76"/>
-      <c r="E165" s="76"/>
-      <c r="F165" s="76"/>
+      <c r="B165" s="56"/>
+      <c r="C165" s="56"/>
+      <c r="D165" s="56"/>
+      <c r="E165" s="56"/>
+      <c r="F165" s="56"/>
     </row>
     <row r="166" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B166" s="76"/>
-      <c r="C166" s="76"/>
-      <c r="D166" s="76"/>
-      <c r="E166" s="76"/>
-      <c r="F166" s="76"/>
+      <c r="B166" s="56"/>
+      <c r="C166" s="56"/>
+      <c r="D166" s="56"/>
+      <c r="E166" s="56"/>
+      <c r="F166" s="56"/>
     </row>
     <row r="169" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B169" s="53" t="s">
+      <c r="B169" s="55" t="s">
         <v>142</v>
       </c>
-      <c r="C169" s="53"/>
-      <c r="D169" s="53"/>
-      <c r="E169" s="53"/>
-      <c r="F169" s="53"/>
+      <c r="C169" s="55"/>
+      <c r="D169" s="55"/>
+      <c r="E169" s="55"/>
+      <c r="F169" s="55"/>
     </row>
     <row r="170" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B170" s="77" t="s">
+      <c r="B170" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="C170" s="77"/>
-      <c r="D170" s="77"/>
-      <c r="E170" s="61" t="s">
+      <c r="C170" s="66"/>
+      <c r="D170" s="66"/>
+      <c r="E170" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="F170" s="61"/>
+      <c r="F170" s="57"/>
     </row>
     <row r="171" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B171" s="77" t="s">
+      <c r="B171" s="66" t="s">
         <v>137</v>
       </c>
-      <c r="C171" s="77"/>
-      <c r="D171" s="77"/>
-      <c r="E171" s="61" t="s">
+      <c r="C171" s="66"/>
+      <c r="D171" s="66"/>
+      <c r="E171" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="F171" s="61"/>
+      <c r="F171" s="57"/>
     </row>
     <row r="172" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="77" t="s">
+      <c r="B172" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="C172" s="77"/>
-      <c r="D172" s="77"/>
-      <c r="E172" s="61" t="s">
+      <c r="C172" s="66"/>
+      <c r="D172" s="66"/>
+      <c r="E172" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="F172" s="61"/>
+      <c r="F172" s="57"/>
     </row>
     <row r="173" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B173" s="77" t="s">
+      <c r="B173" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="C173" s="77"/>
-      <c r="D173" s="77"/>
-      <c r="E173" s="61">
+      <c r="C173" s="66"/>
+      <c r="D173" s="66"/>
+      <c r="E173" s="57">
         <v>4</v>
       </c>
-      <c r="F173" s="61"/>
+      <c r="F173" s="57"/>
     </row>
     <row r="174" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B174" s="75"/>
-      <c r="C174" s="76"/>
-      <c r="D174" s="76"/>
-      <c r="E174" s="76"/>
-      <c r="F174" s="76"/>
+      <c r="B174" s="56"/>
+      <c r="C174" s="56"/>
+      <c r="D174" s="56"/>
+      <c r="E174" s="56"/>
+      <c r="F174" s="56"/>
     </row>
     <row r="175" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B175" s="76"/>
-      <c r="C175" s="76"/>
-      <c r="D175" s="76"/>
-      <c r="E175" s="76"/>
-      <c r="F175" s="76"/>
+      <c r="B175" s="56"/>
+      <c r="C175" s="56"/>
+      <c r="D175" s="56"/>
+      <c r="E175" s="56"/>
+      <c r="F175" s="56"/>
     </row>
     <row r="176" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="76"/>
-      <c r="C176" s="76"/>
-      <c r="D176" s="76"/>
-      <c r="E176" s="76"/>
-      <c r="F176" s="76"/>
+      <c r="B176" s="56"/>
+      <c r="C176" s="56"/>
+      <c r="D176" s="56"/>
+      <c r="E176" s="56"/>
+      <c r="F176" s="56"/>
     </row>
     <row r="177" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B177" s="76"/>
-      <c r="C177" s="76"/>
-      <c r="D177" s="76"/>
-      <c r="E177" s="76"/>
-      <c r="F177" s="76"/>
+      <c r="B177" s="56"/>
+      <c r="C177" s="56"/>
+      <c r="D177" s="56"/>
+      <c r="E177" s="56"/>
+      <c r="F177" s="56"/>
     </row>
     <row r="178" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B178" s="76"/>
-      <c r="C178" s="76"/>
-      <c r="D178" s="76"/>
-      <c r="E178" s="76"/>
-      <c r="F178" s="76"/>
+      <c r="B178" s="56"/>
+      <c r="C178" s="56"/>
+      <c r="D178" s="56"/>
+      <c r="E178" s="56"/>
+      <c r="F178" s="56"/>
     </row>
     <row r="179" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B179" s="76"/>
-      <c r="C179" s="76"/>
-      <c r="D179" s="76"/>
-      <c r="E179" s="76"/>
-      <c r="F179" s="76"/>
+      <c r="B179" s="56"/>
+      <c r="C179" s="56"/>
+      <c r="D179" s="56"/>
+      <c r="E179" s="56"/>
+      <c r="F179" s="56"/>
     </row>
     <row r="180" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B180" s="76"/>
-      <c r="C180" s="76"/>
-      <c r="D180" s="76"/>
-      <c r="E180" s="76"/>
-      <c r="F180" s="76"/>
+      <c r="B180" s="56"/>
+      <c r="C180" s="56"/>
+      <c r="D180" s="56"/>
+      <c r="E180" s="56"/>
+      <c r="F180" s="56"/>
     </row>
     <row r="181" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="182" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B182" s="53" t="s">
+      <c r="B182" s="55" t="s">
         <v>143</v>
       </c>
-      <c r="C182" s="53"/>
-      <c r="D182" s="53"/>
-      <c r="E182" s="53"/>
-      <c r="F182" s="53"/>
+      <c r="C182" s="55"/>
+      <c r="D182" s="55"/>
+      <c r="E182" s="55"/>
+      <c r="F182" s="55"/>
     </row>
     <row r="183" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B183" s="77" t="s">
+      <c r="B183" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="C183" s="77"/>
-      <c r="D183" s="77"/>
-      <c r="E183" s="64" t="s">
+      <c r="C183" s="66"/>
+      <c r="D183" s="66"/>
+      <c r="E183" s="60" t="s">
         <v>136</v>
       </c>
-      <c r="F183" s="65"/>
+      <c r="F183" s="61"/>
     </row>
     <row r="184" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B184" s="77" t="s">
+      <c r="B184" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="C184" s="77"/>
-      <c r="D184" s="77"/>
-      <c r="E184" s="66" t="s">
+      <c r="C184" s="66"/>
+      <c r="D184" s="66"/>
+      <c r="E184" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="F184" s="67"/>
+      <c r="F184" s="63"/>
     </row>
     <row r="185" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B185" s="77" t="s">
+      <c r="B185" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="C185" s="77"/>
-      <c r="D185" s="77"/>
-      <c r="E185" s="62">
+      <c r="C185" s="66"/>
+      <c r="D185" s="66"/>
+      <c r="E185" s="58">
         <v>1</v>
       </c>
-      <c r="F185" s="63"/>
+      <c r="F185" s="59"/>
     </row>
     <row r="186" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B186" s="75"/>
-      <c r="C186" s="76"/>
-      <c r="D186" s="76"/>
-      <c r="E186" s="76"/>
-      <c r="F186" s="76"/>
+      <c r="B186" s="56"/>
+      <c r="C186" s="56"/>
+      <c r="D186" s="56"/>
+      <c r="E186" s="56"/>
+      <c r="F186" s="56"/>
     </row>
     <row r="187" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B187" s="76"/>
-      <c r="C187" s="76"/>
-      <c r="D187" s="76"/>
-      <c r="E187" s="76"/>
-      <c r="F187" s="76"/>
+      <c r="B187" s="56"/>
+      <c r="C187" s="56"/>
+      <c r="D187" s="56"/>
+      <c r="E187" s="56"/>
+      <c r="F187" s="56"/>
     </row>
     <row r="188" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B188" s="76"/>
-      <c r="C188" s="76"/>
-      <c r="D188" s="76"/>
-      <c r="E188" s="76"/>
-      <c r="F188" s="76"/>
+      <c r="B188" s="56"/>
+      <c r="C188" s="56"/>
+      <c r="D188" s="56"/>
+      <c r="E188" s="56"/>
+      <c r="F188" s="56"/>
     </row>
     <row r="189" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B189" s="76"/>
-      <c r="C189" s="76"/>
-      <c r="D189" s="76"/>
-      <c r="E189" s="76"/>
-      <c r="F189" s="76"/>
+      <c r="B189" s="56"/>
+      <c r="C189" s="56"/>
+      <c r="D189" s="56"/>
+      <c r="E189" s="56"/>
+      <c r="F189" s="56"/>
     </row>
     <row r="190" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B190" s="76"/>
-      <c r="C190" s="76"/>
-      <c r="D190" s="76"/>
-      <c r="E190" s="76"/>
-      <c r="F190" s="76"/>
+      <c r="B190" s="56"/>
+      <c r="C190" s="56"/>
+      <c r="D190" s="56"/>
+      <c r="E190" s="56"/>
+      <c r="F190" s="56"/>
     </row>
     <row r="191" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B191" s="76"/>
-      <c r="C191" s="76"/>
-      <c r="D191" s="76"/>
-      <c r="E191" s="76"/>
-      <c r="F191" s="76"/>
+      <c r="B191" s="56"/>
+      <c r="C191" s="56"/>
+      <c r="D191" s="56"/>
+      <c r="E191" s="56"/>
+      <c r="F191" s="56"/>
     </row>
     <row r="192" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B192" s="76"/>
-      <c r="C192" s="76"/>
-      <c r="D192" s="76"/>
-      <c r="E192" s="76"/>
-      <c r="F192" s="76"/>
+      <c r="B192" s="56"/>
+      <c r="C192" s="56"/>
+      <c r="D192" s="56"/>
+      <c r="E192" s="56"/>
+      <c r="F192" s="56"/>
     </row>
     <row r="193" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="194" spans="1:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B194" s="53" t="s">
+      <c r="B194" s="55" t="s">
         <v>145</v>
       </c>
-      <c r="C194" s="53"/>
-      <c r="D194" s="53"/>
-      <c r="E194" s="53"/>
-      <c r="F194" s="53"/>
+      <c r="C194" s="55"/>
+      <c r="D194" s="55"/>
+      <c r="E194" s="55"/>
+      <c r="F194" s="55"/>
     </row>
     <row r="195" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B195" s="77" t="s">
+      <c r="B195" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="C195" s="77"/>
-      <c r="D195" s="77"/>
-      <c r="E195" s="64" t="s">
+      <c r="C195" s="66"/>
+      <c r="D195" s="66"/>
+      <c r="E195" s="60" t="s">
         <v>146</v>
       </c>
-      <c r="F195" s="65"/>
+      <c r="F195" s="61"/>
     </row>
     <row r="196" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B196" s="77" t="s">
+      <c r="B196" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="C196" s="77"/>
-      <c r="D196" s="77"/>
-      <c r="E196" s="66" t="s">
+      <c r="C196" s="66"/>
+      <c r="D196" s="66"/>
+      <c r="E196" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="F196" s="67"/>
+      <c r="F196" s="63"/>
     </row>
     <row r="197" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B197" s="77" t="s">
+      <c r="B197" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="C197" s="77"/>
-      <c r="D197" s="77"/>
-      <c r="E197" s="62">
+      <c r="C197" s="66"/>
+      <c r="D197" s="66"/>
+      <c r="E197" s="58">
         <v>1</v>
       </c>
-      <c r="F197" s="63"/>
+      <c r="F197" s="59"/>
     </row>
     <row r="198" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B198" s="75"/>
-      <c r="C198" s="76"/>
-      <c r="D198" s="76"/>
-      <c r="E198" s="76"/>
-      <c r="F198" s="76"/>
+      <c r="B198" s="56"/>
+      <c r="C198" s="56"/>
+      <c r="D198" s="56"/>
+      <c r="E198" s="56"/>
+      <c r="F198" s="56"/>
     </row>
     <row r="199" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B199" s="76"/>
-      <c r="C199" s="76"/>
-      <c r="D199" s="76"/>
-      <c r="E199" s="76"/>
-      <c r="F199" s="76"/>
+      <c r="B199" s="56"/>
+      <c r="C199" s="56"/>
+      <c r="D199" s="56"/>
+      <c r="E199" s="56"/>
+      <c r="F199" s="56"/>
     </row>
     <row r="200" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B200" s="76"/>
-      <c r="C200" s="76"/>
-      <c r="D200" s="76"/>
-      <c r="E200" s="76"/>
-      <c r="F200" s="76"/>
+      <c r="B200" s="56"/>
+      <c r="C200" s="56"/>
+      <c r="D200" s="56"/>
+      <c r="E200" s="56"/>
+      <c r="F200" s="56"/>
     </row>
     <row r="201" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B201" s="76"/>
-      <c r="C201" s="76"/>
-      <c r="D201" s="76"/>
-      <c r="E201" s="76"/>
-      <c r="F201" s="76"/>
+      <c r="B201" s="56"/>
+      <c r="C201" s="56"/>
+      <c r="D201" s="56"/>
+      <c r="E201" s="56"/>
+      <c r="F201" s="56"/>
     </row>
     <row r="202" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B202" s="76"/>
-      <c r="C202" s="76"/>
-      <c r="D202" s="76"/>
-      <c r="E202" s="76"/>
-      <c r="F202" s="76"/>
+      <c r="B202" s="56"/>
+      <c r="C202" s="56"/>
+      <c r="D202" s="56"/>
+      <c r="E202" s="56"/>
+      <c r="F202" s="56"/>
     </row>
     <row r="203" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B203" s="76"/>
-      <c r="C203" s="76"/>
-      <c r="D203" s="76"/>
-      <c r="E203" s="76"/>
-      <c r="F203" s="76"/>
+      <c r="B203" s="56"/>
+      <c r="C203" s="56"/>
+      <c r="D203" s="56"/>
+      <c r="E203" s="56"/>
+      <c r="F203" s="56"/>
     </row>
     <row r="204" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B204" s="76"/>
-      <c r="C204" s="76"/>
-      <c r="D204" s="76"/>
-      <c r="E204" s="76"/>
-      <c r="F204" s="76"/>
+      <c r="B204" s="56"/>
+      <c r="C204" s="56"/>
+      <c r="D204" s="56"/>
+      <c r="E204" s="56"/>
+      <c r="F204" s="56"/>
     </row>
     <row r="207" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="9" t="s">
@@ -4916,133 +4745,133 @@
       </c>
     </row>
     <row r="209" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B209" s="68" t="s">
+      <c r="B209" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="C209" s="69"/>
-      <c r="D209" s="72" t="s">
+      <c r="C209" s="65"/>
+      <c r="D209" s="69" t="s">
         <v>150</v>
       </c>
-      <c r="E209" s="73"/>
-      <c r="F209" s="74"/>
+      <c r="E209" s="70"/>
+      <c r="F209" s="71"/>
     </row>
     <row r="210" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B210" s="68" t="s">
+      <c r="B210" s="64" t="s">
         <v>151</v>
       </c>
-      <c r="C210" s="69"/>
-      <c r="D210" s="72" t="s">
+      <c r="C210" s="65"/>
+      <c r="D210" s="69" t="s">
         <v>152</v>
       </c>
-      <c r="E210" s="73"/>
-      <c r="F210" s="74"/>
+      <c r="E210" s="70"/>
+      <c r="F210" s="71"/>
     </row>
     <row r="211" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B211" s="68" t="s">
+      <c r="B211" s="64" t="s">
         <v>153</v>
       </c>
-      <c r="C211" s="69"/>
-      <c r="D211" s="72">
+      <c r="C211" s="65"/>
+      <c r="D211" s="69">
         <v>1998</v>
       </c>
-      <c r="E211" s="73"/>
-      <c r="F211" s="74"/>
+      <c r="E211" s="70"/>
+      <c r="F211" s="71"/>
     </row>
     <row r="212" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B212" s="68" t="s">
+      <c r="B212" s="64" t="s">
         <v>154</v>
       </c>
-      <c r="C212" s="69"/>
-      <c r="D212" s="72">
+      <c r="C212" s="65"/>
+      <c r="D212" s="69">
         <v>26</v>
       </c>
-      <c r="E212" s="73"/>
-      <c r="F212" s="74"/>
+      <c r="E212" s="70"/>
+      <c r="F212" s="71"/>
     </row>
     <row r="213" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B213" s="68" t="s">
+      <c r="B213" s="64" t="s">
         <v>155</v>
       </c>
-      <c r="C213" s="69"/>
-      <c r="D213" s="72" t="s">
+      <c r="C213" s="65"/>
+      <c r="D213" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="E213" s="73"/>
-      <c r="F213" s="74"/>
+      <c r="E213" s="70"/>
+      <c r="F213" s="71"/>
     </row>
     <row r="214" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B214" s="68" t="s">
+      <c r="B214" s="64" t="s">
         <v>157</v>
       </c>
-      <c r="C214" s="69"/>
-      <c r="D214" s="72" t="s">
+      <c r="C214" s="65"/>
+      <c r="D214" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="E214" s="73"/>
-      <c r="F214" s="74"/>
+      <c r="E214" s="70"/>
+      <c r="F214" s="71"/>
     </row>
     <row r="215" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B215" s="54"/>
-      <c r="C215" s="55"/>
-      <c r="D215" s="55"/>
-      <c r="E215" s="55"/>
+      <c r="B215" s="56"/>
+      <c r="C215" s="56"/>
+      <c r="D215" s="56"/>
+      <c r="E215" s="56"/>
       <c r="F215" s="56"/>
     </row>
     <row r="216" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B216" s="39"/>
-      <c r="C216" s="57"/>
-      <c r="D216" s="57"/>
-      <c r="E216" s="57"/>
-      <c r="F216" s="40"/>
+      <c r="B216" s="56"/>
+      <c r="C216" s="56"/>
+      <c r="D216" s="56"/>
+      <c r="E216" s="56"/>
+      <c r="F216" s="56"/>
     </row>
     <row r="217" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B217" s="39"/>
-      <c r="C217" s="57"/>
-      <c r="D217" s="57"/>
-      <c r="E217" s="57"/>
-      <c r="F217" s="40"/>
+      <c r="B217" s="56"/>
+      <c r="C217" s="56"/>
+      <c r="D217" s="56"/>
+      <c r="E217" s="56"/>
+      <c r="F217" s="56"/>
     </row>
     <row r="218" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B218" s="39"/>
-      <c r="C218" s="57"/>
-      <c r="D218" s="57"/>
-      <c r="E218" s="57"/>
-      <c r="F218" s="40"/>
+      <c r="B218" s="56"/>
+      <c r="C218" s="56"/>
+      <c r="D218" s="56"/>
+      <c r="E218" s="56"/>
+      <c r="F218" s="56"/>
     </row>
     <row r="219" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B219" s="39"/>
-      <c r="C219" s="57"/>
-      <c r="D219" s="57"/>
-      <c r="E219" s="57"/>
-      <c r="F219" s="40"/>
+      <c r="B219" s="56"/>
+      <c r="C219" s="56"/>
+      <c r="D219" s="56"/>
+      <c r="E219" s="56"/>
+      <c r="F219" s="56"/>
     </row>
     <row r="220" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B220" s="39"/>
-      <c r="C220" s="57"/>
-      <c r="D220" s="57"/>
-      <c r="E220" s="57"/>
-      <c r="F220" s="40"/>
+      <c r="B220" s="56"/>
+      <c r="C220" s="56"/>
+      <c r="D220" s="56"/>
+      <c r="E220" s="56"/>
+      <c r="F220" s="56"/>
     </row>
     <row r="221" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B221" s="39"/>
-      <c r="C221" s="57"/>
-      <c r="D221" s="57"/>
-      <c r="E221" s="57"/>
-      <c r="F221" s="40"/>
+      <c r="B221" s="56"/>
+      <c r="C221" s="56"/>
+      <c r="D221" s="56"/>
+      <c r="E221" s="56"/>
+      <c r="F221" s="56"/>
     </row>
     <row r="222" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B222" s="39"/>
-      <c r="C222" s="57"/>
-      <c r="D222" s="57"/>
-      <c r="E222" s="57"/>
-      <c r="F222" s="40"/>
+      <c r="B222" s="56"/>
+      <c r="C222" s="56"/>
+      <c r="D222" s="56"/>
+      <c r="E222" s="56"/>
+      <c r="F222" s="56"/>
     </row>
     <row r="223" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B223" s="58"/>
-      <c r="C223" s="59"/>
-      <c r="D223" s="59"/>
-      <c r="E223" s="59"/>
-      <c r="F223" s="60"/>
+      <c r="B223" s="56"/>
+      <c r="C223" s="56"/>
+      <c r="D223" s="56"/>
+      <c r="E223" s="56"/>
+      <c r="F223" s="56"/>
     </row>
     <row r="225" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B225" s="10" t="s">
@@ -5050,62 +4879,62 @@
       </c>
     </row>
     <row r="226" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B226" s="68" t="s">
+      <c r="B226" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="C226" s="69"/>
-      <c r="D226" s="72"/>
-      <c r="E226" s="73"/>
-      <c r="F226" s="74"/>
+      <c r="C226" s="65"/>
+      <c r="D226" s="69"/>
+      <c r="E226" s="70"/>
+      <c r="F226" s="71"/>
     </row>
     <row r="227" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B227" s="79"/>
-      <c r="C227" s="55"/>
-      <c r="D227" s="55"/>
-      <c r="E227" s="55"/>
-      <c r="F227" s="56"/>
+      <c r="B227" s="73"/>
+      <c r="C227" s="74"/>
+      <c r="D227" s="74"/>
+      <c r="E227" s="74"/>
+      <c r="F227" s="75"/>
     </row>
     <row r="228" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B228" s="39"/>
-      <c r="C228" s="57"/>
-      <c r="D228" s="57"/>
-      <c r="E228" s="57"/>
-      <c r="F228" s="40"/>
+      <c r="B228" s="41"/>
+      <c r="C228" s="76"/>
+      <c r="D228" s="76"/>
+      <c r="E228" s="76"/>
+      <c r="F228" s="42"/>
     </row>
     <row r="229" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B229" s="39"/>
-      <c r="C229" s="57"/>
-      <c r="D229" s="57"/>
-      <c r="E229" s="57"/>
-      <c r="F229" s="40"/>
+      <c r="B229" s="41"/>
+      <c r="C229" s="76"/>
+      <c r="D229" s="76"/>
+      <c r="E229" s="76"/>
+      <c r="F229" s="42"/>
     </row>
     <row r="230" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B230" s="39"/>
-      <c r="C230" s="57"/>
-      <c r="D230" s="57"/>
-      <c r="E230" s="57"/>
-      <c r="F230" s="40"/>
+      <c r="B230" s="41"/>
+      <c r="C230" s="76"/>
+      <c r="D230" s="76"/>
+      <c r="E230" s="76"/>
+      <c r="F230" s="42"/>
     </row>
     <row r="231" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B231" s="39"/>
-      <c r="C231" s="57"/>
-      <c r="D231" s="57"/>
-      <c r="E231" s="57"/>
-      <c r="F231" s="40"/>
+      <c r="B231" s="41"/>
+      <c r="C231" s="76"/>
+      <c r="D231" s="76"/>
+      <c r="E231" s="76"/>
+      <c r="F231" s="42"/>
     </row>
     <row r="232" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B232" s="39"/>
-      <c r="C232" s="57"/>
-      <c r="D232" s="57"/>
-      <c r="E232" s="57"/>
-      <c r="F232" s="40"/>
+      <c r="B232" s="41"/>
+      <c r="C232" s="76"/>
+      <c r="D232" s="76"/>
+      <c r="E232" s="76"/>
+      <c r="F232" s="42"/>
     </row>
     <row r="233" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B233" s="58"/>
-      <c r="C233" s="59"/>
-      <c r="D233" s="59"/>
-      <c r="E233" s="59"/>
-      <c r="F233" s="60"/>
+      <c r="B233" s="77"/>
+      <c r="C233" s="78"/>
+      <c r="D233" s="78"/>
+      <c r="E233" s="78"/>
+      <c r="F233" s="79"/>
     </row>
     <row r="235" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B235" s="10" t="s">
@@ -5113,82 +4942,82 @@
       </c>
     </row>
     <row r="236" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B236" s="68" t="s">
+      <c r="B236" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="C236" s="69"/>
-      <c r="D236" s="72" t="s">
+      <c r="C236" s="65"/>
+      <c r="D236" s="69" t="s">
         <v>161</v>
       </c>
-      <c r="E236" s="73"/>
-      <c r="F236" s="74"/>
+      <c r="E236" s="70"/>
+      <c r="F236" s="71"/>
     </row>
     <row r="237" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B237" s="68" t="s">
+      <c r="B237" s="64" t="s">
         <v>162</v>
       </c>
-      <c r="C237" s="69"/>
-      <c r="D237" s="72"/>
-      <c r="E237" s="73"/>
-      <c r="F237" s="74"/>
+      <c r="C237" s="65"/>
+      <c r="D237" s="69"/>
+      <c r="E237" s="70"/>
+      <c r="F237" s="71"/>
     </row>
     <row r="238" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B238" s="79"/>
-      <c r="C238" s="55"/>
-      <c r="D238" s="55"/>
-      <c r="E238" s="55"/>
-      <c r="F238" s="56"/>
+      <c r="B238" s="73"/>
+      <c r="C238" s="74"/>
+      <c r="D238" s="74"/>
+      <c r="E238" s="74"/>
+      <c r="F238" s="75"/>
     </row>
     <row r="239" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B239" s="39"/>
-      <c r="C239" s="57"/>
-      <c r="D239" s="57"/>
-      <c r="E239" s="57"/>
-      <c r="F239" s="40"/>
+      <c r="B239" s="41"/>
+      <c r="C239" s="76"/>
+      <c r="D239" s="76"/>
+      <c r="E239" s="76"/>
+      <c r="F239" s="42"/>
     </row>
     <row r="240" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B240" s="39"/>
-      <c r="C240" s="57"/>
-      <c r="D240" s="57"/>
-      <c r="E240" s="57"/>
-      <c r="F240" s="40"/>
+      <c r="B240" s="41"/>
+      <c r="C240" s="76"/>
+      <c r="D240" s="76"/>
+      <c r="E240" s="76"/>
+      <c r="F240" s="42"/>
     </row>
     <row r="241" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B241" s="39"/>
-      <c r="C241" s="57"/>
-      <c r="D241" s="57"/>
-      <c r="E241" s="57"/>
-      <c r="F241" s="40"/>
+      <c r="B241" s="41"/>
+      <c r="C241" s="76"/>
+      <c r="D241" s="76"/>
+      <c r="E241" s="76"/>
+      <c r="F241" s="42"/>
     </row>
     <row r="242" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B242" s="39"/>
-      <c r="C242" s="57"/>
-      <c r="D242" s="57"/>
-      <c r="E242" s="57"/>
-      <c r="F242" s="40"/>
+      <c r="B242" s="41"/>
+      <c r="C242" s="76"/>
+      <c r="D242" s="76"/>
+      <c r="E242" s="76"/>
+      <c r="F242" s="42"/>
     </row>
     <row r="243" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B243" s="39"/>
-      <c r="C243" s="57"/>
-      <c r="D243" s="57"/>
-      <c r="E243" s="57"/>
-      <c r="F243" s="40"/>
+      <c r="B243" s="41"/>
+      <c r="C243" s="76"/>
+      <c r="D243" s="76"/>
+      <c r="E243" s="76"/>
+      <c r="F243" s="42"/>
     </row>
     <row r="244" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B244" s="58"/>
-      <c r="C244" s="59"/>
-      <c r="D244" s="59"/>
-      <c r="E244" s="59"/>
-      <c r="F244" s="60"/>
+      <c r="B244" s="77"/>
+      <c r="C244" s="78"/>
+      <c r="D244" s="78"/>
+      <c r="E244" s="78"/>
+      <c r="F244" s="79"/>
     </row>
     <row r="245" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B245" s="68" t="s">
+      <c r="B245" s="64" t="s">
         <v>163</v>
       </c>
-      <c r="C245" s="69"/>
-      <c r="D245" s="72"/>
-      <c r="E245" s="73"/>
-      <c r="F245" s="74"/>
+      <c r="C245" s="65"/>
+      <c r="D245" s="69"/>
+      <c r="E245" s="70"/>
+      <c r="F245" s="71"/>
     </row>
     <row r="248" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B248" s="10" t="s">
@@ -5196,64 +5025,64 @@
       </c>
     </row>
     <row r="249" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B249" s="68" t="s">
+      <c r="B249" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="C249" s="69"/>
-      <c r="D249" s="72" t="s">
+      <c r="C249" s="65"/>
+      <c r="D249" s="69" t="s">
         <v>165</v>
       </c>
-      <c r="E249" s="73"/>
-      <c r="F249" s="74"/>
+      <c r="E249" s="70"/>
+      <c r="F249" s="71"/>
     </row>
     <row r="250" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B250" s="54"/>
-      <c r="C250" s="55"/>
-      <c r="D250" s="55"/>
-      <c r="E250" s="55"/>
+      <c r="B250" s="56"/>
+      <c r="C250" s="56"/>
+      <c r="D250" s="56"/>
+      <c r="E250" s="56"/>
       <c r="F250" s="56"/>
     </row>
     <row r="251" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B251" s="39"/>
-      <c r="C251" s="57"/>
-      <c r="D251" s="57"/>
-      <c r="E251" s="57"/>
-      <c r="F251" s="40"/>
+      <c r="B251" s="56"/>
+      <c r="C251" s="56"/>
+      <c r="D251" s="56"/>
+      <c r="E251" s="56"/>
+      <c r="F251" s="56"/>
     </row>
     <row r="252" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B252" s="39"/>
-      <c r="C252" s="57"/>
-      <c r="D252" s="57"/>
-      <c r="E252" s="57"/>
-      <c r="F252" s="40"/>
+      <c r="B252" s="56"/>
+      <c r="C252" s="56"/>
+      <c r="D252" s="56"/>
+      <c r="E252" s="56"/>
+      <c r="F252" s="56"/>
     </row>
     <row r="253" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B253" s="39"/>
-      <c r="C253" s="57"/>
-      <c r="D253" s="57"/>
-      <c r="E253" s="57"/>
-      <c r="F253" s="40"/>
+      <c r="B253" s="56"/>
+      <c r="C253" s="56"/>
+      <c r="D253" s="56"/>
+      <c r="E253" s="56"/>
+      <c r="F253" s="56"/>
     </row>
     <row r="254" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B254" s="39"/>
-      <c r="C254" s="57"/>
-      <c r="D254" s="57"/>
-      <c r="E254" s="57"/>
-      <c r="F254" s="40"/>
+      <c r="B254" s="56"/>
+      <c r="C254" s="56"/>
+      <c r="D254" s="56"/>
+      <c r="E254" s="56"/>
+      <c r="F254" s="56"/>
     </row>
     <row r="255" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B255" s="39"/>
-      <c r="C255" s="57"/>
-      <c r="D255" s="57"/>
-      <c r="E255" s="57"/>
-      <c r="F255" s="40"/>
+      <c r="B255" s="56"/>
+      <c r="C255" s="56"/>
+      <c r="D255" s="56"/>
+      <c r="E255" s="56"/>
+      <c r="F255" s="56"/>
     </row>
     <row r="256" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B256" s="58"/>
-      <c r="C256" s="59"/>
-      <c r="D256" s="59"/>
-      <c r="E256" s="59"/>
-      <c r="F256" s="60"/>
+      <c r="B256" s="56"/>
+      <c r="C256" s="56"/>
+      <c r="D256" s="56"/>
+      <c r="E256" s="56"/>
+      <c r="F256" s="56"/>
     </row>
     <row r="258" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B258" s="10" t="s">
@@ -5261,64 +5090,64 @@
       </c>
     </row>
     <row r="259" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B259" s="68" t="s">
+      <c r="B259" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="C259" s="69"/>
-      <c r="D259" s="72" t="s">
+      <c r="C259" s="65"/>
+      <c r="D259" s="69" t="s">
         <v>167</v>
       </c>
-      <c r="E259" s="73"/>
-      <c r="F259" s="74"/>
+      <c r="E259" s="70"/>
+      <c r="F259" s="71"/>
     </row>
     <row r="260" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B260" s="54"/>
-      <c r="C260" s="55"/>
-      <c r="D260" s="55"/>
-      <c r="E260" s="55"/>
+      <c r="B260" s="56"/>
+      <c r="C260" s="56"/>
+      <c r="D260" s="56"/>
+      <c r="E260" s="56"/>
       <c r="F260" s="56"/>
     </row>
     <row r="261" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B261" s="39"/>
-      <c r="C261" s="57"/>
-      <c r="D261" s="57"/>
-      <c r="E261" s="57"/>
-      <c r="F261" s="40"/>
+      <c r="B261" s="56"/>
+      <c r="C261" s="56"/>
+      <c r="D261" s="56"/>
+      <c r="E261" s="56"/>
+      <c r="F261" s="56"/>
     </row>
     <row r="262" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B262" s="39"/>
-      <c r="C262" s="57"/>
-      <c r="D262" s="57"/>
-      <c r="E262" s="57"/>
-      <c r="F262" s="40"/>
+      <c r="B262" s="56"/>
+      <c r="C262" s="56"/>
+      <c r="D262" s="56"/>
+      <c r="E262" s="56"/>
+      <c r="F262" s="56"/>
     </row>
     <row r="263" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B263" s="39"/>
-      <c r="C263" s="57"/>
-      <c r="D263" s="57"/>
-      <c r="E263" s="57"/>
-      <c r="F263" s="40"/>
+      <c r="B263" s="56"/>
+      <c r="C263" s="56"/>
+      <c r="D263" s="56"/>
+      <c r="E263" s="56"/>
+      <c r="F263" s="56"/>
     </row>
     <row r="264" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B264" s="39"/>
-      <c r="C264" s="57"/>
-      <c r="D264" s="57"/>
-      <c r="E264" s="57"/>
-      <c r="F264" s="40"/>
+      <c r="B264" s="56"/>
+      <c r="C264" s="56"/>
+      <c r="D264" s="56"/>
+      <c r="E264" s="56"/>
+      <c r="F264" s="56"/>
     </row>
     <row r="265" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B265" s="39"/>
-      <c r="C265" s="57"/>
-      <c r="D265" s="57"/>
-      <c r="E265" s="57"/>
-      <c r="F265" s="40"/>
+      <c r="B265" s="56"/>
+      <c r="C265" s="56"/>
+      <c r="D265" s="56"/>
+      <c r="E265" s="56"/>
+      <c r="F265" s="56"/>
     </row>
     <row r="266" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B266" s="58"/>
-      <c r="C266" s="59"/>
-      <c r="D266" s="59"/>
-      <c r="E266" s="59"/>
-      <c r="F266" s="60"/>
+      <c r="B266" s="56"/>
+      <c r="C266" s="56"/>
+      <c r="D266" s="56"/>
+      <c r="E266" s="56"/>
+      <c r="F266" s="56"/>
     </row>
     <row r="268" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="9" t="s">
@@ -5326,75 +5155,75 @@
       </c>
     </row>
     <row r="269" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B269" s="68" t="s">
+      <c r="B269" s="64" t="s">
         <v>169</v>
       </c>
-      <c r="C269" s="69"/>
-      <c r="D269" s="72">
+      <c r="C269" s="65"/>
+      <c r="D269" s="69">
         <v>6</v>
       </c>
-      <c r="E269" s="73"/>
-      <c r="F269" s="74"/>
+      <c r="E269" s="70"/>
+      <c r="F269" s="71"/>
     </row>
     <row r="270" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B270" s="68" t="s">
+      <c r="B270" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="C270" s="69"/>
-      <c r="D270" s="72" t="s">
+      <c r="C270" s="65"/>
+      <c r="D270" s="69" t="s">
         <v>171</v>
       </c>
-      <c r="E270" s="73"/>
-      <c r="F270" s="74"/>
+      <c r="E270" s="70"/>
+      <c r="F270" s="71"/>
     </row>
     <row r="271" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B271" s="54"/>
-      <c r="C271" s="55"/>
-      <c r="D271" s="55"/>
-      <c r="E271" s="55"/>
+      <c r="B271" s="56"/>
+      <c r="C271" s="56"/>
+      <c r="D271" s="56"/>
+      <c r="E271" s="56"/>
       <c r="F271" s="56"/>
     </row>
     <row r="272" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B272" s="39"/>
-      <c r="C272" s="57"/>
-      <c r="D272" s="57"/>
-      <c r="E272" s="57"/>
-      <c r="F272" s="40"/>
+      <c r="B272" s="56"/>
+      <c r="C272" s="56"/>
+      <c r="D272" s="56"/>
+      <c r="E272" s="56"/>
+      <c r="F272" s="56"/>
     </row>
     <row r="273" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B273" s="39"/>
-      <c r="C273" s="57"/>
-      <c r="D273" s="57"/>
-      <c r="E273" s="57"/>
-      <c r="F273" s="40"/>
+      <c r="B273" s="56"/>
+      <c r="C273" s="56"/>
+      <c r="D273" s="56"/>
+      <c r="E273" s="56"/>
+      <c r="F273" s="56"/>
     </row>
     <row r="274" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B274" s="39"/>
-      <c r="C274" s="57"/>
-      <c r="D274" s="57"/>
-      <c r="E274" s="57"/>
-      <c r="F274" s="40"/>
+      <c r="B274" s="56"/>
+      <c r="C274" s="56"/>
+      <c r="D274" s="56"/>
+      <c r="E274" s="56"/>
+      <c r="F274" s="56"/>
     </row>
     <row r="275" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B275" s="39"/>
-      <c r="C275" s="57"/>
-      <c r="D275" s="57"/>
-      <c r="E275" s="57"/>
-      <c r="F275" s="40"/>
+      <c r="B275" s="56"/>
+      <c r="C275" s="56"/>
+      <c r="D275" s="56"/>
+      <c r="E275" s="56"/>
+      <c r="F275" s="56"/>
     </row>
     <row r="276" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B276" s="39"/>
-      <c r="C276" s="57"/>
-      <c r="D276" s="57"/>
-      <c r="E276" s="57"/>
-      <c r="F276" s="40"/>
+      <c r="B276" s="56"/>
+      <c r="C276" s="56"/>
+      <c r="D276" s="56"/>
+      <c r="E276" s="56"/>
+      <c r="F276" s="56"/>
     </row>
     <row r="277" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B277" s="58"/>
-      <c r="C277" s="59"/>
-      <c r="D277" s="59"/>
-      <c r="E277" s="59"/>
-      <c r="F277" s="60"/>
+      <c r="B277" s="56"/>
+      <c r="C277" s="56"/>
+      <c r="D277" s="56"/>
+      <c r="E277" s="56"/>
+      <c r="F277" s="56"/>
     </row>
     <row r="281" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" s="9" t="s">
@@ -5411,10 +5240,10 @@
       <c r="C283" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="D283" s="89" t="s">
+      <c r="D283" s="90" t="s">
         <v>174</v>
       </c>
-      <c r="E283" s="89"/>
+      <c r="E283" s="90"/>
       <c r="F283" s="20" t="s">
         <v>175</v>
       </c>
@@ -5432,10 +5261,10 @@
       <c r="C284" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="D284" s="50">
+      <c r="D284" s="52">
         <v>2.5</v>
       </c>
-      <c r="E284" s="51"/>
+      <c r="E284" s="53"/>
       <c r="F284" s="21" t="s">
         <v>177</v>
       </c>
@@ -5453,10 +5282,10 @@
       <c r="C285" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="D285" s="50">
+      <c r="D285" s="52">
         <v>2.5</v>
       </c>
-      <c r="E285" s="51"/>
+      <c r="E285" s="53"/>
       <c r="F285" s="21" t="s">
         <v>178</v>
       </c>
@@ -5474,10 +5303,10 @@
       <c r="C286" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="D286" s="50">
+      <c r="D286" s="52">
         <v>2.5</v>
       </c>
-      <c r="E286" s="51"/>
+      <c r="E286" s="53"/>
       <c r="F286" s="21" t="s">
         <v>179</v>
       </c>
@@ -5495,10 +5324,10 @@
       <c r="C287" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="D287" s="50" t="s">
+      <c r="D287" s="52" t="s">
         <v>180</v>
       </c>
-      <c r="E287" s="51"/>
+      <c r="E287" s="53"/>
       <c r="F287" s="21" t="s">
         <v>181</v>
       </c>
@@ -5516,10 +5345,10 @@
       <c r="C288" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="D288" s="50">
+      <c r="D288" s="52">
         <v>2.5</v>
       </c>
-      <c r="E288" s="51"/>
+      <c r="E288" s="53"/>
       <c r="F288" s="21" t="s">
         <v>182</v>
       </c>
@@ -5537,10 +5366,10 @@
       <c r="C289" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="D289" s="50">
+      <c r="D289" s="52">
         <v>2.5</v>
       </c>
-      <c r="E289" s="51"/>
+      <c r="E289" s="53"/>
       <c r="F289" s="21" t="s">
         <v>183</v>
       </c>
@@ -5558,10 +5387,10 @@
       <c r="C290" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="D290" s="50">
+      <c r="D290" s="52">
         <v>2.5</v>
       </c>
-      <c r="E290" s="51"/>
+      <c r="E290" s="53"/>
       <c r="F290" s="21" t="s">
         <v>185</v>
       </c>
@@ -5579,10 +5408,10 @@
       <c r="C291" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="D291" s="50">
+      <c r="D291" s="52">
         <v>2.5</v>
       </c>
-      <c r="E291" s="51"/>
+      <c r="E291" s="53"/>
       <c r="F291" s="21" t="s">
         <v>186</v>
       </c>
@@ -5600,10 +5429,10 @@
       <c r="C292" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="D292" s="50">
+      <c r="D292" s="52">
         <v>2.5</v>
       </c>
-      <c r="E292" s="51"/>
+      <c r="E292" s="53"/>
       <c r="F292" s="21" t="s">
         <v>187</v>
       </c>
@@ -5621,10 +5450,10 @@
       <c r="C293" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="D293" s="50">
+      <c r="D293" s="52">
         <v>2.5</v>
       </c>
-      <c r="E293" s="51"/>
+      <c r="E293" s="53"/>
       <c r="F293" s="21" t="s">
         <v>188</v>
       </c>
@@ -5642,10 +5471,10 @@
       <c r="C294" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="D294" s="50">
+      <c r="D294" s="52">
         <v>2.5</v>
       </c>
-      <c r="E294" s="51"/>
+      <c r="E294" s="53"/>
       <c r="F294" s="21" t="s">
         <v>189</v>
       </c>
@@ -5663,10 +5492,10 @@
       <c r="C295" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="D295" s="50">
+      <c r="D295" s="52">
         <v>2.5</v>
       </c>
-      <c r="E295" s="51"/>
+      <c r="E295" s="53"/>
       <c r="F295" s="21" t="s">
         <v>190</v>
       </c>
@@ -5684,10 +5513,10 @@
       <c r="C296" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="D296" s="50">
+      <c r="D296" s="52">
         <v>2.5</v>
       </c>
-      <c r="E296" s="51"/>
+      <c r="E296" s="53"/>
       <c r="F296" s="21" t="s">
         <v>191</v>
       </c>
@@ -5701,10 +5530,10 @@
         <v>47</v>
       </c>
       <c r="C297" s="22"/>
-      <c r="D297" s="50" t="s">
+      <c r="D297" s="52" t="s">
         <v>192</v>
       </c>
-      <c r="E297" s="51"/>
+      <c r="E297" s="53"/>
       <c r="F297" s="21" t="s">
         <v>193</v>
       </c>
@@ -5719,61 +5548,61 @@
       </c>
     </row>
     <row r="345" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B345" s="90" t="s">
+      <c r="B345" s="91" t="s">
         <v>195</v>
       </c>
-      <c r="C345" s="90"/>
-      <c r="D345" s="90"/>
-      <c r="E345" s="90"/>
-      <c r="F345" s="90"/>
+      <c r="C345" s="91"/>
+      <c r="D345" s="91"/>
+      <c r="E345" s="91"/>
+      <c r="F345" s="91"/>
     </row>
     <row r="347" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B347" s="86" t="s">
+      <c r="B347" s="87" t="s">
         <v>196</v>
       </c>
-      <c r="C347" s="87"/>
-      <c r="D347" s="87"/>
-      <c r="E347" s="87"/>
-      <c r="F347" s="88"/>
+      <c r="C347" s="88"/>
+      <c r="D347" s="88"/>
+      <c r="E347" s="88"/>
+      <c r="F347" s="89"/>
     </row>
     <row r="348" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B348" s="91"/>
-      <c r="C348" s="87"/>
-      <c r="D348" s="87"/>
-      <c r="E348" s="87"/>
-      <c r="F348" s="88"/>
+      <c r="B348" s="56"/>
+      <c r="C348" s="56"/>
+      <c r="D348" s="56"/>
+      <c r="E348" s="56"/>
+      <c r="F348" s="56"/>
     </row>
     <row r="349" spans="1:6" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B349" s="91"/>
-      <c r="C349" s="87"/>
-      <c r="D349" s="87"/>
-      <c r="E349" s="87"/>
-      <c r="F349" s="88"/>
+      <c r="B349" s="56"/>
+      <c r="C349" s="56"/>
+      <c r="D349" s="56"/>
+      <c r="E349" s="56"/>
+      <c r="F349" s="56"/>
     </row>
     <row r="352" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B352" s="86" t="s">
+      <c r="B352" s="87" t="s">
         <v>197</v>
       </c>
-      <c r="C352" s="87"/>
-      <c r="D352" s="87"/>
-      <c r="E352" s="87"/>
-      <c r="F352" s="88"/>
+      <c r="C352" s="88"/>
+      <c r="D352" s="88"/>
+      <c r="E352" s="88"/>
+      <c r="F352" s="89"/>
     </row>
     <row r="353" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B353" s="86" t="s">
+      <c r="B353" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C353" s="87"/>
-      <c r="D353" s="87"/>
-      <c r="E353" s="87"/>
-      <c r="F353" s="88"/>
+      <c r="C353" s="88"/>
+      <c r="D353" s="88"/>
+      <c r="E353" s="88"/>
+      <c r="F353" s="89"/>
     </row>
     <row r="354" spans="2:6" ht="141" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B354" s="86"/>
-      <c r="C354" s="87"/>
-      <c r="D354" s="87"/>
-      <c r="E354" s="87"/>
-      <c r="F354" s="88"/>
+      <c r="B354" s="87"/>
+      <c r="C354" s="88"/>
+      <c r="D354" s="88"/>
+      <c r="E354" s="88"/>
+      <c r="F354" s="89"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -5993,29 +5822,8 @@
     <mergeCell ref="D291:E291"/>
     <mergeCell ref="D292:E292"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B348" r:id="rId1" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPSjA5QjNaQnZPbW1SbHh5NTE0TnI5eVRKUDNUdDJMVEVhRGRza2YzUHhiUHhaU25qdjJWRGw4K1FRUmREcGZSS1ZwT0U2YmhWQUkzYjQ3Vm1vdEJXVkU9?name="/>
-    <hyperlink ref="B349" r:id="rId2" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPSjA5QjNaQnZPbW1SbHh5NTE0TnI5eVRKUDNUdDJMVEVhRGRza2YzUHhiUHhaU25qdjJWRGw4K1FRUmREcGZSS1ZwT0U2YmhWQUkzYjQ3Vm1vdEJXVkU9?name="/>
-    <hyperlink ref="A38" r:id="rId3" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPUDBraUFjbk84RUZBdWpLbnhUTlhFMVdDQ014Y09RdjVFdUtnN0w4SHJQQWMxb1VUUTRoUXhhZUZES1pFbkdKYktaYmFyZUxnYmw1RktZelRrWkRSNkk9?name="/>
-    <hyperlink ref="E38" r:id="rId4" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPUDBraUFjbk84RUZBdWpLbnhUTlhFMVdDQ014Y09RdjVFdUtnN0w4SHJQQUVjYUg4MG9ZcE1BSUtmVUhKcWxRQW53MER6Y1lFWDBuSzFwalR5RGd6UHM9?name="/>
-    <hyperlink ref="A50" r:id="rId5" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPUDBraUFjbk84RUZBdWpLbnhUTlhFMVdDQ014Y09RdjVFdUtnN0w4SHJQQVh5NzU3ZzZxS0RubW1NTHRuemxwbU42KzIzNGNmczdDdE1OUktpc3Q2bUE9?name="/>
-    <hyperlink ref="E50" r:id="rId6" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPUDBraUFjbk84RUZBdWpLbnhUTlhFMVdDQ014Y09RdjVFdUtnN0w4SHJQQVFSZ2UzS01wUmcwbEpyVy9URzR0UWVKbnhJUWNvMkV1Y0lTQ1BBZnpjQUk9?name="/>
-    <hyperlink ref="B215" r:id="rId7" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUlBJKzBDcm96YzJRaUx3UFZCUHkrdldBMkUyaDdCeWNBNm5uZS9QZGc4WjA9?name="/>
-    <hyperlink ref="B250" r:id="rId8" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUjVOa1RlWXBmMmZSeWFnUmIwWlVtVklOL2tnUkx2VjNaMXplYXA2YTdmaHM9?name="/>
-    <hyperlink ref="B260" r:id="rId9" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUk42bWhRL3E3cE1BckVZSXdqWFYyL0tZTkpnN1BtYVpJUWtpQTM2ajZWMFU9?name="/>
-    <hyperlink ref="B271" r:id="rId10" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUk42bWhRL3E3cE1BckVZSXdqWFYyL00zekdrcGp4NlhIRHVYcG9vY0RoMWs9?name="/>
-    <hyperlink ref="B67" r:id="rId11" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPUDBraUFjbk84RUZBdWpLbnhUTlhFMVdDQ014Y09RdjVFdUtnN0w4SHJQQWxOaWNsVS9HMXNNMldoWFBtK0E4emtWVGU4U0dLL0lSTE96TTZGYmV5WHc9?name="/>
-    <hyperlink ref="B83" r:id="rId12" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPUDBraUFjbk84RUZBdWpLbnhUTlhFMVdDQ014Y09RdjVFdUtnN0w4SHJQQS9NeEJuaEJwb2RQdksvdDc3YWtMVlJESUUxMEU3YUpPb09SQkdyWmtqN0U9?name="/>
-    <hyperlink ref="B99" r:id="rId13" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPUDBraUFjbk84RUZBdWpLbnhUTlhFMVdDQ014Y09RdjVFdUtnN0w4SHJQQU9lUGl4bWdsZFFCRXNJZW02cldROUNucDM4RDYwQjhhS24xTzdYNzl2STg9?name="/>
-    <hyperlink ref="B131" r:id="rId14" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUkpWYlAwdUIzclpWMkVMZWVWbUlLTkpHSVFoUWlEdXRhenRqdGxCaXlERGc9?name="/>
-    <hyperlink ref="B147" r:id="rId15" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUjVUVklIa0R5eDlaMzV1RWNRdzNaTDlqS3V2MnQrb2s2NlFMUGxtdE96WnM9?name="/>
-    <hyperlink ref="B160" r:id="rId16" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUkhUUER5dURYcWtEOHI1ZnQyRzNyK3QvR2xoOEc3cmduQUV1U1J6ZThpTFU9?name="/>
-    <hyperlink ref="B174" r:id="rId17" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUm9VRXk3cC9mczE3c2poa2lMN3JCcnJCUjF4TE4wTTgvUmduTHFtenpMbEE9?name="/>
-    <hyperlink ref="B186" r:id="rId18" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUnJqMWtya09tVG05Tm1OeERjdmp3L3Y5dXJ2cXFIMHNEamlrYWFaY0gvd2s9?name="/>
-    <hyperlink ref="B198" r:id="rId19" display="https://forms.kizeo.com/data/medias/secure/dm9lY2pPdEpBdGo4QkJyMy8reEtPQjYydXVOdnMzMlVlZzgrb3lCNG42N3p2TW54SWljOEtqUjV2WVNiZExSUi93OEk0MjNmUWRvR25Ud2tDQWliNHpNa3dUNUQ5SDZhNTBVemRwRExsd3c9?name="/>
-  </hyperlinks>
   <pageMargins left="0.39370078740157" right="0.39370078740157" top="0.78740157480314998" bottom="0.51181102362205" header="0.31496062992126" footer="0.27559055118109999"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;"Segoe UI Semibold,Normal"&amp;10Audit énergétique 2023&amp;R&amp;"Segoe UI Semibold,Normal"&amp;10&amp;P / &amp;N</oddFooter>
@@ -6027,7 +5835,7 @@
     <brk id="246" man="1"/>
     <brk id="279" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId21"/>
-  <legacyDrawingHF r:id="rId22"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawingHF r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v0.0.16.13 xlsx 11 safe +1
</commit_message>
<xml_diff>
--- a/ERapp/static/Kizeo.xlsx
+++ b/ERapp/static/Kizeo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="113">
   <si>
     <t>Données générales</t>
   </si>
@@ -34,54 +34,30 @@
     <t>Date de visite</t>
   </si>
   <si>
-    <t>06/10/2023</t>
-  </si>
-  <si>
     <t>Adresse</t>
   </si>
   <si>
-    <t>5 impasse Medicis</t>
-  </si>
-  <si>
     <t>Code postal</t>
   </si>
   <si>
     <t>Ville</t>
   </si>
   <si>
-    <t>Toulouse</t>
-  </si>
-  <si>
     <t>Année de construction</t>
   </si>
   <si>
-    <t>Entre 1949 et 1974</t>
-  </si>
-  <si>
     <t>Nom du client</t>
   </si>
   <si>
-    <t>FAZZINI Pier-Francesco</t>
-  </si>
-  <si>
     <t>Téléphone</t>
   </si>
   <si>
-    <t>0624001049</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>p.f.fazzini@gmail.com</t>
-  </si>
-  <si>
     <t>Numéro fiscal</t>
   </si>
   <si>
-    <t>1001284113053</t>
-  </si>
-  <si>
     <t>Référénce d'avis</t>
   </si>
   <si>
@@ -94,9 +70,6 @@
     <t>Preuve SHAB</t>
   </si>
   <si>
-    <t>Mesurée</t>
-  </si>
-  <si>
     <t>SHAB ajouté depuis 15 ans</t>
   </si>
   <si>
@@ -163,65 +136,10 @@
     <t>Cuisine</t>
   </si>
   <si>
-    <t>Non</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porte-fenêtre avec soubassement, 2 vantaux, pvc, double vitrage , volets bois
-Porte de service donnant sur un espace non chauffé, bois plein
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.40
-0.80
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.35
-2.10
-</t>
-  </si>
-  <si>
-    <t>1
-1
-0</t>
-  </si>
-  <si>
     <t>Dégagement 1</t>
   </si>
   <si>
-    <t>Oui</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porte d'entrée, double vitrage (Inférieur à 60%) ,pvc
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.90
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.15
-</t>
-  </si>
-  <si>
-    <t>1
-0
-0</t>
-  </si>
-  <si>
     <t>W.C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fenêtre 1 vantail, pvc, double vitrage, volets bois
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.50
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.75
-</t>
   </si>
   <si>
     <t>Salle d'eau</t>
@@ -231,49 +149,15 @@
 </t>
   </si>
   <si>
-    <t>0
-0
-0</t>
-  </si>
-  <si>
     <t>Séjour</t>
   </si>
   <si>
-    <t xml:space="preserve">Porte-fenêtre avec soubassement, 2 vantaux, pvc, double vitrage , volets bois
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.40
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.35
-</t>
-  </si>
-  <si>
-    <t>2
-0
-0</t>
-  </si>
-  <si>
     <t>Salle d'étude</t>
   </si>
   <si>
-    <t xml:space="preserve">Fenêtre, 2 vantaux, pvc, double vitrage , volets bois
-</t>
-  </si>
-  <si>
     <t>Salle de bain</t>
   </si>
   <si>
-    <t xml:space="preserve">Fenêtre, 1 vantail, pvc, double vitrage
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.20
-</t>
-  </si>
-  <si>
     <t>Chambre 1</t>
   </si>
   <si>
@@ -292,21 +176,6 @@
     <t>Cage d'escalier</t>
   </si>
   <si>
-    <t xml:space="preserve">Fenêtre, 1 vantail, pvc, double vitrage , volets bois
-Pavée de verres (rdc)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.60
-0.60
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.65
-1.25
-</t>
-  </si>
-  <si>
     <t>RAPPORT D'AUDIT ENERGETIQUE</t>
   </si>
   <si>
@@ -316,9 +185,6 @@
     <t>BUREAU D'ETUDE</t>
   </si>
   <si>
-    <t>Adiabati.Green</t>
-  </si>
-  <si>
     <t>Date de la visite</t>
   </si>
   <si>
@@ -349,66 +215,24 @@
     <t>Etat d'occupation</t>
   </si>
   <si>
-    <t>Plus de 2 ans</t>
-  </si>
-  <si>
     <t>Surface habitable [m²]</t>
   </si>
   <si>
     <t>FAÇADES</t>
   </si>
   <si>
-    <t>Sud-Ouest</t>
-  </si>
-  <si>
-    <t>Nord-Est</t>
-  </si>
-  <si>
-    <t>Pas de mitoyenneté</t>
-  </si>
-  <si>
-    <t>Longueur = 11 m</t>
-  </si>
-  <si>
-    <t>Hauteur = 5.45 m</t>
-  </si>
-  <si>
-    <t>Surface = 51.75 m²</t>
-  </si>
-  <si>
-    <t>Nord-Ouest</t>
-  </si>
-  <si>
-    <t>Sud-Est</t>
-  </si>
-  <si>
-    <t>Longueur = 7.10 m</t>
-  </si>
-  <si>
-    <t>Surface = 38.70 m²</t>
-  </si>
-  <si>
     <t>CARACTÉRISTIQUES DE L'ENVELOPPE</t>
   </si>
   <si>
-    <t>Murs - Type 1 - L'extérieur</t>
-  </si>
-  <si>
     <t>Composition</t>
   </si>
   <si>
-    <t>Briques creuses</t>
-  </si>
-  <si>
     <t>Ep. Mur (cm)</t>
   </si>
   <si>
     <t>Isolation</t>
   </si>
   <si>
-    <t>Non isolé</t>
-  </si>
-  <si>
     <t>Ep. Isolant (cm)</t>
   </si>
   <si>
@@ -418,21 +242,12 @@
     <t>Commentaires</t>
   </si>
   <si>
-    <t>Murs - Type 2 - LNC</t>
-  </si>
-  <si>
     <t>Plancher bas - Type 1</t>
   </si>
   <si>
     <t>Position</t>
   </si>
   <si>
-    <t>Terre plein</t>
-  </si>
-  <si>
-    <t>Dalle béton</t>
-  </si>
-  <si>
     <t>Surface (m²)</t>
   </si>
   <si>
@@ -448,36 +263,18 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Combles perdus</t>
-  </si>
-  <si>
-    <t>ITE</t>
-  </si>
-  <si>
-    <t>Plus de 10 ans</t>
-  </si>
-  <si>
     <t>Plancher haut - Type 2</t>
   </si>
   <si>
     <t>Fenêtre battante</t>
   </si>
   <si>
-    <t>PVC</t>
-  </si>
-  <si>
     <t>Type de vitrage</t>
   </si>
   <si>
-    <t>Double vitrage</t>
-  </si>
-  <si>
     <t>Volets</t>
   </si>
   <si>
-    <t>Battant bois</t>
-  </si>
-  <si>
     <t>Nombre</t>
   </si>
   <si>
@@ -487,33 +284,18 @@
     <t>Portes - Type 1</t>
   </si>
   <si>
-    <t>Avec &lt;30% de vitrage simple</t>
-  </si>
-  <si>
     <t>Portes - Type 2</t>
   </si>
   <si>
-    <t>Bois</t>
-  </si>
-  <si>
-    <t>Opaque pleine simple</t>
-  </si>
-  <si>
     <t>SYSTÈMES TECHNIQUES</t>
   </si>
   <si>
     <t>CHAUFFAGE PRINCIPAL</t>
   </si>
   <si>
-    <t>Chaudière gaz Standard</t>
-  </si>
-  <si>
     <t>Marque de chaudière</t>
   </si>
   <si>
-    <t>FRISQUET</t>
-  </si>
-  <si>
     <t>Année de mise en œuvre</t>
   </si>
   <si>
@@ -523,24 +305,15 @@
     <t>Type d'émetteur</t>
   </si>
   <si>
-    <t>Radiateur fonte</t>
-  </si>
-  <si>
     <t>Type de régulation</t>
   </si>
   <si>
-    <t>Robinet thermostatique</t>
-  </si>
-  <si>
     <t>CHAUFFAGE D'APPOINT</t>
   </si>
   <si>
     <t>EAU CHAUDE SANITAIRE</t>
   </si>
   <si>
-    <t>Liée au système de chauffage</t>
-  </si>
-  <si>
     <t>Volume (L)</t>
   </si>
   <si>
@@ -550,15 +323,9 @@
     <t>VENTILATION</t>
   </si>
   <si>
-    <t>VMC Autoréglable</t>
-  </si>
-  <si>
     <t>CLIMATISATION</t>
   </si>
   <si>
-    <t>PAC Air/Air</t>
-  </si>
-  <si>
     <t>COMPTEUR ÉLÉCTRIQUE</t>
   </si>
   <si>
@@ -568,9 +335,6 @@
     <t>Puissance souscrite (kVA)</t>
   </si>
   <si>
-    <t>Monophasé</t>
-  </si>
-  <si>
     <t>CARACTERISTIQUES DES PIECES</t>
   </si>
   <si>
@@ -581,62 +345,10 @@
   </si>
   <si>
     <t>Longueur x Largeur</t>
-  </si>
-  <si>
-    <t>RDC</t>
-  </si>
-  <si>
-    <t>2.56x3.85</t>
-  </si>
-  <si>
-    <t>6.40x1.48</t>
-  </si>
-  <si>
-    <t>0.90x1.50</t>
-  </si>
-  <si>
-    <t>2.50
-1.60</t>
-  </si>
-  <si>
-    <t>2.80x1.58</t>
-  </si>
-  <si>
-    <t>7.56x3.85</t>
-  </si>
-  <si>
-    <t>2.95x2.70</t>
-  </si>
-  <si>
-    <t>RDC+1</t>
-  </si>
-  <si>
-    <t>2.90x1.70</t>
-  </si>
-  <si>
-    <t>3.58x3.55</t>
-  </si>
-  <si>
-    <t>3.90x2.92</t>
-  </si>
-  <si>
-    <t>3.55x3.53</t>
-  </si>
-  <si>
-    <t>1.37x1.00</t>
-  </si>
-  <si>
-    <t>1.60x2.30</t>
-  </si>
-  <si>
-    <t>0x0</t>
   </si>
   <si>
     <t xml:space="preserve">
 </t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>AVIS DE PASSAGE</t>
@@ -655,7 +367,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -727,6 +439,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1063,7 +781,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1331,6 +1049,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1737,115 +1458,89 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3">
-        <v>31200</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="3">
-        <v>2</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="3">
-        <v>103</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3"/>
     </row>
@@ -1862,9 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1879,19 +1572,19 @@
   <sheetData>
     <row r="1" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K1" s="34" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="L1" s="35"/>
       <c r="M1" s="35"/>
       <c r="N1" s="35"/>
       <c r="O1" s="36"/>
       <c r="P1" s="30" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="Q1" s="31"/>
       <c r="R1" s="31"/>
       <c r="T1" s="37" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="U1" s="38"/>
       <c r="V1" s="38"/>
@@ -1899,67 +1592,67 @@
     </row>
     <row r="2" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="29"/>
       <c r="D2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="N2" s="32" t="s">
         <v>31</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" s="32" t="s">
-        <v>40</v>
       </c>
       <c r="O2" s="33"/>
       <c r="P2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="V2" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="W2" s="13" t="s">
         <v>36</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="U2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="V2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1967,26 +1660,14 @@
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="H3" s="3">
-        <v>2.56</v>
-      </c>
-      <c r="I3" s="3">
-        <v>3.85</v>
-      </c>
-      <c r="J3" s="3">
-        <v>9.86</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -1996,97 +1677,51 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
-      <c r="T3" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="U3" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="V3" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="W3" s="17" t="s">
-        <v>51</v>
-      </c>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="92"/>
+      <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="24"/>
       <c r="C4" s="25"/>
       <c r="D4" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="H4" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1.48</v>
-      </c>
-      <c r="J4" s="3">
-        <v>9.4700000000000006</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="3">
-        <v>1.47</v>
-      </c>
+      <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
-      <c r="R4" s="3">
-        <v>0.85</v>
-      </c>
-      <c r="S4" s="3">
-        <v>8.6199999999999992</v>
-      </c>
-      <c r="T4" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="U4" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="V4" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="W4" s="17" t="s">
-        <v>57</v>
-      </c>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="92"/>
     </row>
     <row r="5" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="24"/>
       <c r="C5" s="25"/>
       <c r="D5" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="I5" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1.35</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -2096,156 +1731,82 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
-      <c r="T5" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="U5" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="V5" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="W5" s="17" t="s">
-        <v>57</v>
-      </c>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
     </row>
     <row r="6" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="24"/>
       <c r="C6" s="25"/>
       <c r="D6" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>53</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3">
-        <v>2.8</v>
-      </c>
-      <c r="I6" s="3">
-        <v>1.58</v>
-      </c>
-      <c r="J6" s="3">
-        <v>4.42</v>
-      </c>
-      <c r="K6" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="L6" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="N6" s="3">
-        <v>3.03</v>
-      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
       <c r="O6" s="3"/>
-      <c r="P6" s="3">
-        <v>1</v>
-      </c>
+      <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
-      <c r="R6" s="3">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="S6" s="3">
-        <v>3.84</v>
-      </c>
-      <c r="T6" s="17" t="s">
-        <v>63</v>
-      </c>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="17"/>
       <c r="U6" s="17" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="V6" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="W6" s="17" t="s">
-        <v>64</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="W6" s="17"/>
     </row>
     <row r="7" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="24"/>
       <c r="C7" s="25"/>
       <c r="D7" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="H7" s="3">
-        <v>7.56</v>
-      </c>
-      <c r="I7" s="3">
-        <v>3.85</v>
-      </c>
-      <c r="J7" s="3">
-        <v>29.11</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="P7" s="3">
-        <v>3.59</v>
-      </c>
+      <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
-      <c r="R7" s="3">
-        <v>1.62</v>
-      </c>
-      <c r="S7" s="3">
-        <v>27.49</v>
-      </c>
-      <c r="T7" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="U7" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="V7" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="W7" s="17" t="s">
-        <v>69</v>
-      </c>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
     </row>
     <row r="8" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
       <c r="D8" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="H8" s="3">
-        <v>2.95</v>
-      </c>
-      <c r="I8" s="3">
-        <v>2.7</v>
-      </c>
-      <c r="J8" s="3">
-        <v>7.97</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -2255,150 +1816,78 @@
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
-      <c r="T8" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="U8" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="V8" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="W8" s="17" t="s">
-        <v>57</v>
-      </c>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
     </row>
     <row r="9" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="24"/>
       <c r="C9" s="25"/>
       <c r="D9" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="H9" s="3">
-        <v>2.9</v>
-      </c>
-      <c r="I9" s="3">
-        <v>1.7</v>
-      </c>
-      <c r="J9" s="3">
-        <v>4.93</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="3">
-        <v>0.2</v>
-      </c>
+      <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="3">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="S9" s="3">
-        <v>4.6399999999999997</v>
-      </c>
-      <c r="T9" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="U9" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="V9" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="W9" s="17" t="s">
-        <v>57</v>
-      </c>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
     </row>
     <row r="10" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
       <c r="D10" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="H10" s="3">
-        <v>3.58</v>
-      </c>
-      <c r="I10" s="3">
-        <v>3.55</v>
-      </c>
-      <c r="J10" s="3">
-        <v>12.71</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
-      <c r="P10" s="3">
-        <v>1.37</v>
-      </c>
+      <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="R10" s="3">
-        <v>0.92</v>
-      </c>
-      <c r="S10" s="3">
-        <v>11.79</v>
-      </c>
-      <c r="T10" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="U10" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="V10" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="W10" s="17" t="s">
-        <v>57</v>
-      </c>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
     </row>
     <row r="11" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="24"/>
       <c r="C11" s="25"/>
       <c r="D11" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="H11" s="3">
-        <v>3.9</v>
-      </c>
-      <c r="I11" s="3">
-        <v>2.92</v>
-      </c>
-      <c r="J11" s="3">
-        <v>11.39</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -2408,97 +1897,51 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
-      <c r="T11" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="U11" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="V11" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="W11" s="17" t="s">
-        <v>57</v>
-      </c>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
     </row>
     <row r="12" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
       <c r="D12" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="H12" s="3">
-        <v>3.55</v>
-      </c>
-      <c r="I12" s="3">
-        <v>3.53</v>
-      </c>
-      <c r="J12" s="3">
-        <v>12.53</v>
-      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="3">
-        <v>0.6</v>
-      </c>
+      <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="S12" s="3">
-        <v>11.93</v>
-      </c>
-      <c r="T12" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="U12" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="V12" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="W12" s="17" t="s">
-        <v>57</v>
-      </c>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
     </row>
     <row r="13" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
       <c r="D13" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="H13" s="3">
-        <v>1.37</v>
-      </c>
-      <c r="I13" s="3">
-        <v>1</v>
-      </c>
-      <c r="J13" s="3">
-        <v>1.37</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -2509,96 +1952,62 @@
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="17" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="U13" s="17" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="V13" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="W13" s="17" t="s">
-        <v>64</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="W13" s="17"/>
     </row>
     <row r="14" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="24"/>
       <c r="C14" s="25"/>
       <c r="D14" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="H14" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="I14" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="J14" s="3">
-        <v>3.68</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-      <c r="P14" s="3">
-        <v>0.6</v>
-      </c>
+      <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="R14" s="3">
-        <v>0.78</v>
-      </c>
-      <c r="S14" s="3">
-        <v>2.9</v>
-      </c>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
       <c r="T14" s="17" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="U14" s="17" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="V14" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="W14" s="17" t="s">
-        <v>64</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="W14" s="17"/>
     </row>
     <row r="15" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3">
-        <v>0</v>
-      </c>
-      <c r="J15" s="3">
-        <v>0</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
@@ -2608,36 +2017,22 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="U15" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="V15" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="W15" s="17" t="s">
-        <v>51</v>
-      </c>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
     </row>
     <row r="16" spans="1:23" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
       <c r="D16" s="23"/>
-      <c r="E16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="3">
-        <v>0</v>
-      </c>
+      <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -2648,17 +2043,15 @@
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="17" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="U16" s="17" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="V16" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="W16" s="17" t="s">
-        <v>64</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="W16" s="17"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -2678,8 +2071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" view="pageLayout" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" view="pageLayout" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -2694,7 +2087,7 @@
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
@@ -2734,45 +2127,35 @@
     <row r="24" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="50" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="C25" s="51"/>
       <c r="D25" s="6"/>
       <c r="E25" s="50" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="F25" s="51"/>
     </row>
     <row r="26" spans="2:6" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="42" t="s">
-        <v>13</v>
-      </c>
+      <c r="B26" s="42"/>
       <c r="C26" s="43"/>
-      <c r="E26" s="46" t="s">
-        <v>87</v>
-      </c>
+      <c r="E26" s="46"/>
       <c r="F26" s="47"/>
     </row>
     <row r="27" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="40" t="s">
-        <v>6</v>
-      </c>
+      <c r="B27" s="40"/>
       <c r="C27" s="41"/>
       <c r="E27" s="40"/>
       <c r="F27" s="41"/>
     </row>
     <row r="28" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="42">
-        <v>31200</v>
-      </c>
+      <c r="B28" s="42"/>
       <c r="C28" s="43"/>
       <c r="E28" s="42"/>
       <c r="F28" s="43"/>
     </row>
     <row r="29" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="44" t="s">
-        <v>9</v>
-      </c>
+      <c r="B29" s="44"/>
       <c r="C29" s="45"/>
       <c r="E29" s="44"/>
       <c r="F29" s="45"/>
@@ -2781,19 +2164,17 @@
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C32" s="7" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="8" t="s">
-        <v>4</v>
-      </c>
+      <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
     </row>
@@ -2802,7 +2183,7 @@
     <row r="36" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="39" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="C37" s="39"/>
       <c r="D37" s="39"/>
@@ -2848,7 +2229,7 @@
   <dimension ref="A3:K354"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A7" sqref="A7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2867,7 +2248,7 @@
   <sheetData>
     <row r="3" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="89" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="B3" s="89"/>
       <c r="C3" s="89"/>
@@ -2878,12 +2259,12 @@
     </row>
     <row r="6" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="90" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="B7" s="90"/>
       <c r="C7" s="90"/>
@@ -2894,7 +2275,7 @@
     </row>
     <row r="25" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2902,99 +2283,73 @@
     </row>
     <row r="27" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="91" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="C27" s="91"/>
       <c r="D27" s="91"/>
-      <c r="E27" s="91" t="s">
-        <v>11</v>
-      </c>
+      <c r="E27" s="91"/>
       <c r="F27" s="91"/>
     </row>
     <row r="28" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="91" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="C28" s="91"/>
       <c r="D28" s="91"/>
-      <c r="E28" s="91" t="s">
-        <v>98</v>
-      </c>
+      <c r="E28" s="91"/>
       <c r="F28" s="91"/>
     </row>
     <row r="29" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="91" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="C29" s="91"/>
       <c r="D29" s="91"/>
-      <c r="E29" s="91">
-        <v>103</v>
-      </c>
+      <c r="E29" s="91"/>
       <c r="F29" s="91"/>
     </row>
     <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="55" t="s">
-        <v>101</v>
-      </c>
+      <c r="A33" s="55"/>
       <c r="B33" s="55"/>
       <c r="C33" s="55"/>
-      <c r="E33" s="55" t="s">
-        <v>102</v>
-      </c>
+      <c r="E33" s="55"/>
       <c r="F33" s="55"/>
       <c r="G33" s="55"/>
     </row>
     <row r="34" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="78" t="s">
-        <v>103</v>
-      </c>
+      <c r="A34" s="78"/>
       <c r="B34" s="78"/>
       <c r="C34" s="78"/>
-      <c r="E34" s="78" t="s">
-        <v>103</v>
-      </c>
+      <c r="E34" s="78"/>
       <c r="F34" s="78"/>
       <c r="G34" s="78"/>
     </row>
     <row r="35" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="78" t="s">
-        <v>104</v>
-      </c>
+      <c r="A35" s="78"/>
       <c r="B35" s="78"/>
       <c r="C35" s="78"/>
-      <c r="E35" s="78" t="s">
-        <v>104</v>
-      </c>
+      <c r="E35" s="78"/>
       <c r="F35" s="78"/>
       <c r="G35" s="78"/>
     </row>
     <row r="36" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="78" t="s">
-        <v>105</v>
-      </c>
+      <c r="A36" s="78"/>
       <c r="B36" s="78"/>
       <c r="C36" s="78"/>
-      <c r="E36" s="78" t="s">
-        <v>105</v>
-      </c>
+      <c r="E36" s="78"/>
       <c r="F36" s="78"/>
       <c r="G36" s="78"/>
     </row>
     <row r="37" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="78" t="s">
-        <v>106</v>
-      </c>
+      <c r="A37" s="78"/>
       <c r="B37" s="78"/>
       <c r="C37" s="78"/>
-      <c r="E37" s="78" t="s">
-        <v>106</v>
-      </c>
+      <c r="E37" s="78"/>
       <c r="F37" s="78"/>
       <c r="G37" s="78"/>
     </row>
@@ -3056,50 +2411,34 @@
     </row>
     <row r="45" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="55" t="s">
-        <v>107</v>
-      </c>
+      <c r="A46" s="55"/>
       <c r="B46" s="55"/>
       <c r="C46" s="55"/>
-      <c r="E46" s="55" t="s">
-        <v>108</v>
-      </c>
+      <c r="E46" s="55"/>
       <c r="F46" s="55"/>
       <c r="G46" s="55"/>
     </row>
     <row r="47" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="78" t="s">
-        <v>109</v>
-      </c>
+      <c r="A47" s="78"/>
       <c r="B47" s="78"/>
       <c r="C47" s="78"/>
-      <c r="E47" s="78" t="s">
-        <v>109</v>
-      </c>
+      <c r="E47" s="78"/>
       <c r="F47" s="78"/>
       <c r="G47" s="78"/>
     </row>
     <row r="48" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="78" t="s">
-        <v>105</v>
-      </c>
+      <c r="A48" s="78"/>
       <c r="B48" s="78"/>
       <c r="C48" s="78"/>
-      <c r="E48" s="78" t="s">
-        <v>105</v>
-      </c>
+      <c r="E48" s="78"/>
       <c r="F48" s="78"/>
       <c r="G48" s="78"/>
     </row>
     <row r="49" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="78" t="s">
-        <v>110</v>
-      </c>
+      <c r="A49" s="78"/>
       <c r="B49" s="78"/>
       <c r="C49" s="78"/>
-      <c r="E49" s="78" t="s">
-        <v>110</v>
-      </c>
+      <c r="E49" s="78"/>
       <c r="F49" s="78"/>
       <c r="G49" s="78"/>
     </row>
@@ -3163,13 +2502,11 @@
     <row r="58" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="55" t="s">
-        <v>112</v>
-      </c>
+      <c r="B60" s="55"/>
       <c r="C60" s="55"/>
       <c r="D60" s="55"/>
       <c r="E60" s="55"/>
@@ -3177,40 +2514,34 @@
     </row>
     <row r="61" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="68" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="C61" s="69"/>
       <c r="D61" s="70"/>
-      <c r="E61" s="67" t="s">
-        <v>114</v>
-      </c>
+      <c r="E61" s="67"/>
       <c r="F61" s="67"/>
     </row>
     <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="79" t="s">
-        <v>115</v>
+        <v>68</v>
       </c>
       <c r="C62" s="80"/>
       <c r="D62" s="81"/>
-      <c r="E62" s="67">
-        <v>0.3</v>
-      </c>
+      <c r="E62" s="67"/>
       <c r="F62" s="67"/>
     </row>
     <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="68" t="s">
-        <v>116</v>
+        <v>69</v>
       </c>
       <c r="C63" s="69"/>
       <c r="D63" s="70"/>
-      <c r="E63" s="67" t="s">
-        <v>117</v>
-      </c>
+      <c r="E63" s="67"/>
       <c r="F63" s="67"/>
     </row>
     <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="68" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="C64" s="69"/>
       <c r="D64" s="70"/>
@@ -3219,7 +2550,7 @@
     </row>
     <row r="65" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="68" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="C65" s="69"/>
       <c r="D65" s="70"/>
@@ -3228,7 +2559,7 @@
     </row>
     <row r="66" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="68" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="C66" s="69"/>
       <c r="D66" s="70"/>
@@ -3287,9 +2618,7 @@
     <row r="74" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="76" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="55" t="s">
-        <v>121</v>
-      </c>
+      <c r="B76" s="55"/>
       <c r="C76" s="55"/>
       <c r="D76" s="55"/>
       <c r="E76" s="55"/>
@@ -3297,40 +2626,34 @@
     </row>
     <row r="77" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="57" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="C77" s="57"/>
       <c r="D77" s="57"/>
-      <c r="E77" s="67" t="s">
-        <v>114</v>
-      </c>
+      <c r="E77" s="67"/>
       <c r="F77" s="67"/>
     </row>
     <row r="78" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="57" t="s">
-        <v>115</v>
+        <v>68</v>
       </c>
       <c r="C78" s="57"/>
       <c r="D78" s="57"/>
-      <c r="E78" s="67">
-        <v>0.3</v>
-      </c>
+      <c r="E78" s="67"/>
       <c r="F78" s="67"/>
     </row>
     <row r="79" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="57" t="s">
-        <v>116</v>
+        <v>69</v>
       </c>
       <c r="C79" s="57"/>
       <c r="D79" s="57"/>
-      <c r="E79" s="67" t="s">
-        <v>117</v>
-      </c>
+      <c r="E79" s="67"/>
       <c r="F79" s="67"/>
     </row>
     <row r="80" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="57" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="C80" s="57"/>
       <c r="D80" s="57"/>
@@ -3339,7 +2662,7 @@
     </row>
     <row r="81" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="57" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="C81" s="57"/>
       <c r="D81" s="57"/>
@@ -3348,7 +2671,7 @@
     </row>
     <row r="82" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="68" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="C82" s="69"/>
       <c r="D82" s="70"/>
@@ -3407,7 +2730,7 @@
     <row r="90" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="91" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="55" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="C91" s="55"/>
       <c r="D91" s="55"/>
@@ -3416,40 +2739,34 @@
     </row>
     <row r="92" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="57" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
       <c r="C92" s="57"/>
       <c r="D92" s="57"/>
-      <c r="E92" s="76" t="s">
-        <v>124</v>
-      </c>
+      <c r="E92" s="76"/>
       <c r="F92" s="77"/>
     </row>
     <row r="93" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="57" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="C93" s="57"/>
       <c r="D93" s="57"/>
-      <c r="E93" s="73" t="s">
-        <v>125</v>
-      </c>
+      <c r="E93" s="73"/>
       <c r="F93" s="74"/>
     </row>
     <row r="94" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="57" t="s">
-        <v>116</v>
+        <v>69</v>
       </c>
       <c r="C94" s="57"/>
       <c r="D94" s="57"/>
-      <c r="E94" s="73" t="s">
-        <v>117</v>
-      </c>
+      <c r="E94" s="73"/>
       <c r="F94" s="74"/>
     </row>
     <row r="95" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="57" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="C95" s="57"/>
       <c r="D95" s="57"/>
@@ -3458,7 +2775,7 @@
     </row>
     <row r="96" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" s="57" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="C96" s="57"/>
       <c r="D96" s="57"/>
@@ -3467,18 +2784,16 @@
     </row>
     <row r="97" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="57" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="C97" s="57"/>
       <c r="D97" s="57"/>
-      <c r="E97" s="71">
-        <v>62</v>
-      </c>
+      <c r="E97" s="71"/>
       <c r="F97" s="72"/>
     </row>
     <row r="98" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="68" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="C98" s="69"/>
       <c r="D98" s="70"/>
@@ -3537,7 +2852,7 @@
     <row r="106" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="107" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" s="55" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="C107" s="55"/>
       <c r="D107" s="55"/>
@@ -3546,40 +2861,40 @@
     </row>
     <row r="108" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="57" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
       <c r="C108" s="57"/>
       <c r="D108" s="57"/>
       <c r="E108" s="76" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="F108" s="77"/>
     </row>
     <row r="109" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B109" s="57" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="C109" s="57"/>
       <c r="D109" s="57"/>
       <c r="E109" s="73" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="F109" s="74"/>
     </row>
     <row r="110" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B110" s="57" t="s">
-        <v>116</v>
+        <v>69</v>
       </c>
       <c r="C110" s="57"/>
       <c r="D110" s="57"/>
       <c r="E110" s="73" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="F110" s="74"/>
     </row>
     <row r="111" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B111" s="57" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="C111" s="57"/>
       <c r="D111" s="57"/>
@@ -3588,18 +2903,18 @@
     </row>
     <row r="112" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="57" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="C112" s="57"/>
       <c r="D112" s="57"/>
       <c r="E112" s="71" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="F112" s="72"/>
     </row>
     <row r="113" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B113" s="57" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="C113" s="57"/>
       <c r="D113" s="57"/>
@@ -3608,7 +2923,7 @@
     </row>
     <row r="114" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B114" s="68" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="C114" s="69"/>
       <c r="D114" s="70"/>
@@ -3666,7 +2981,7 @@
     </row>
     <row r="123" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B123" s="55" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="C123" s="55"/>
       <c r="D123" s="55"/>
@@ -3675,73 +2990,61 @@
     </row>
     <row r="124" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B124" s="57" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="C124" s="57"/>
       <c r="D124" s="57"/>
-      <c r="E124" s="76" t="s">
-        <v>131</v>
-      </c>
+      <c r="E124" s="76"/>
       <c r="F124" s="77"/>
     </row>
     <row r="125" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B125" s="57" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="C125" s="57"/>
       <c r="D125" s="57"/>
-      <c r="E125" s="73" t="s">
-        <v>125</v>
-      </c>
+      <c r="E125" s="73"/>
       <c r="F125" s="74"/>
     </row>
     <row r="126" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B126" s="57" t="s">
-        <v>116</v>
+        <v>69</v>
       </c>
       <c r="C126" s="57"/>
       <c r="D126" s="57"/>
-      <c r="E126" s="73" t="s">
-        <v>132</v>
-      </c>
+      <c r="E126" s="73"/>
       <c r="F126" s="74"/>
     </row>
     <row r="127" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B127" s="57" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="C127" s="57"/>
       <c r="D127" s="57"/>
-      <c r="E127" s="73">
-        <v>0.06</v>
-      </c>
+      <c r="E127" s="73"/>
       <c r="F127" s="74"/>
     </row>
     <row r="128" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B128" s="57" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="C128" s="57"/>
       <c r="D128" s="57"/>
-      <c r="E128" s="71" t="s">
-        <v>133</v>
-      </c>
+      <c r="E128" s="71"/>
       <c r="F128" s="72"/>
     </row>
     <row r="129" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B129" s="57" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="C129" s="57"/>
       <c r="D129" s="57"/>
-      <c r="E129" s="71">
-        <v>48.75</v>
-      </c>
+      <c r="E129" s="71"/>
       <c r="F129" s="72"/>
     </row>
     <row r="130" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B130" s="68" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="C130" s="69"/>
       <c r="D130" s="70"/>
@@ -3799,7 +3102,7 @@
     </row>
     <row r="139" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B139" s="55" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="C139" s="55"/>
       <c r="D139" s="55"/>
@@ -3808,40 +3111,34 @@
     </row>
     <row r="140" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="57" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="C140" s="57"/>
       <c r="D140" s="57"/>
-      <c r="E140" s="76" t="s">
-        <v>131</v>
-      </c>
+      <c r="E140" s="76"/>
       <c r="F140" s="77"/>
     </row>
     <row r="141" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B141" s="57" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="C141" s="57"/>
       <c r="D141" s="57"/>
-      <c r="E141" s="73" t="s">
-        <v>125</v>
-      </c>
+      <c r="E141" s="73"/>
       <c r="F141" s="74"/>
     </row>
     <row r="142" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B142" s="57" t="s">
-        <v>116</v>
+        <v>69</v>
       </c>
       <c r="C142" s="57"/>
       <c r="D142" s="57"/>
-      <c r="E142" s="73" t="s">
-        <v>117</v>
-      </c>
+      <c r="E142" s="73"/>
       <c r="F142" s="74"/>
     </row>
     <row r="143" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B143" s="57" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="C143" s="57"/>
       <c r="D143" s="57"/>
@@ -3850,7 +3147,7 @@
     </row>
     <row r="144" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B144" s="57" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="C144" s="57"/>
       <c r="D144" s="57"/>
@@ -3859,18 +3156,16 @@
     </row>
     <row r="145" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B145" s="57" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="C145" s="57"/>
       <c r="D145" s="57"/>
-      <c r="E145" s="71">
-        <v>13.25</v>
-      </c>
+      <c r="E145" s="71"/>
       <c r="F145" s="72"/>
     </row>
     <row r="146" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B146" s="68" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="C146" s="69"/>
       <c r="D146" s="70"/>
@@ -3928,7 +3223,7 @@
     </row>
     <row r="155" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B155" s="55" t="s">
-        <v>135</v>
+        <v>81</v>
       </c>
       <c r="C155" s="55"/>
       <c r="D155" s="55"/>
@@ -3937,46 +3232,38 @@
     </row>
     <row r="156" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B156" s="57" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="C156" s="57"/>
       <c r="D156" s="57"/>
-      <c r="E156" s="76" t="s">
-        <v>136</v>
-      </c>
+      <c r="E156" s="76"/>
       <c r="F156" s="77"/>
     </row>
     <row r="157" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B157" s="57" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="C157" s="57"/>
       <c r="D157" s="57"/>
-      <c r="E157" s="73" t="s">
-        <v>138</v>
-      </c>
+      <c r="E157" s="73"/>
       <c r="F157" s="74"/>
     </row>
     <row r="158" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B158" s="57" t="s">
-        <v>139</v>
+        <v>83</v>
       </c>
       <c r="C158" s="57"/>
       <c r="D158" s="57"/>
-      <c r="E158" s="73" t="s">
-        <v>140</v>
-      </c>
+      <c r="E158" s="73"/>
       <c r="F158" s="74"/>
     </row>
     <row r="159" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B159" s="57" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
       <c r="C159" s="57"/>
       <c r="D159" s="57"/>
-      <c r="E159" s="71">
-        <v>6</v>
-      </c>
+      <c r="E159" s="71"/>
       <c r="F159" s="72"/>
     </row>
     <row r="160" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4030,7 +3317,7 @@
     </row>
     <row r="169" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B169" s="55" t="s">
-        <v>142</v>
+        <v>85</v>
       </c>
       <c r="C169" s="55"/>
       <c r="D169" s="55"/>
@@ -4039,46 +3326,38 @@
     </row>
     <row r="170" spans="2:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B170" s="57" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="C170" s="57"/>
       <c r="D170" s="57"/>
-      <c r="E170" s="67" t="s">
-        <v>136</v>
-      </c>
+      <c r="E170" s="67"/>
       <c r="F170" s="67"/>
     </row>
     <row r="171" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B171" s="57" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="C171" s="57"/>
       <c r="D171" s="57"/>
-      <c r="E171" s="67" t="s">
-        <v>138</v>
-      </c>
+      <c r="E171" s="67"/>
       <c r="F171" s="67"/>
     </row>
     <row r="172" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B172" s="57" t="s">
-        <v>139</v>
+        <v>83</v>
       </c>
       <c r="C172" s="57"/>
       <c r="D172" s="57"/>
-      <c r="E172" s="67" t="s">
-        <v>140</v>
-      </c>
+      <c r="E172" s="67"/>
       <c r="F172" s="67"/>
     </row>
     <row r="173" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B173" s="57" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
       <c r="C173" s="57"/>
       <c r="D173" s="57"/>
-      <c r="E173" s="67">
-        <v>4</v>
-      </c>
+      <c r="E173" s="67"/>
       <c r="F173" s="67"/>
     </row>
     <row r="174" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4133,7 +3412,7 @@
     <row r="181" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="182" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B182" s="55" t="s">
-        <v>143</v>
+        <v>86</v>
       </c>
       <c r="C182" s="55"/>
       <c r="D182" s="55"/>
@@ -4142,35 +3421,29 @@
     </row>
     <row r="183" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B183" s="57" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="C183" s="57"/>
       <c r="D183" s="57"/>
-      <c r="E183" s="76" t="s">
-        <v>136</v>
-      </c>
+      <c r="E183" s="76"/>
       <c r="F183" s="77"/>
     </row>
     <row r="184" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B184" s="57" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="C184" s="57"/>
       <c r="D184" s="57"/>
-      <c r="E184" s="73" t="s">
-        <v>144</v>
-      </c>
+      <c r="E184" s="73"/>
       <c r="F184" s="74"/>
     </row>
     <row r="185" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B185" s="57" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
       <c r="C185" s="57"/>
       <c r="D185" s="57"/>
-      <c r="E185" s="71">
-        <v>1</v>
-      </c>
+      <c r="E185" s="71"/>
       <c r="F185" s="72"/>
     </row>
     <row r="186" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -4225,7 +3498,7 @@
     <row r="193" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="194" spans="1:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B194" s="55" t="s">
-        <v>145</v>
+        <v>87</v>
       </c>
       <c r="C194" s="55"/>
       <c r="D194" s="55"/>
@@ -4234,35 +3507,29 @@
     </row>
     <row r="195" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B195" s="57" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="C195" s="57"/>
       <c r="D195" s="57"/>
-      <c r="E195" s="76" t="s">
-        <v>146</v>
-      </c>
+      <c r="E195" s="76"/>
       <c r="F195" s="77"/>
     </row>
     <row r="196" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B196" s="57" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="C196" s="57"/>
       <c r="D196" s="57"/>
-      <c r="E196" s="73" t="s">
-        <v>147</v>
-      </c>
+      <c r="E196" s="73"/>
       <c r="F196" s="74"/>
     </row>
     <row r="197" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B197" s="57" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
       <c r="C197" s="57"/>
       <c r="D197" s="57"/>
-      <c r="E197" s="71">
-        <v>1</v>
-      </c>
+      <c r="E197" s="71"/>
       <c r="F197" s="72"/>
     </row>
     <row r="198" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4316,77 +3583,65 @@
     </row>
     <row r="207" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="9" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
     </row>
     <row r="208" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B208" s="10" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
     </row>
     <row r="209" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B209" s="61" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="C209" s="62"/>
-      <c r="D209" s="63" t="s">
-        <v>150</v>
-      </c>
+      <c r="D209" s="63"/>
       <c r="E209" s="64"/>
       <c r="F209" s="65"/>
     </row>
     <row r="210" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B210" s="61" t="s">
-        <v>151</v>
+        <v>90</v>
       </c>
       <c r="C210" s="62"/>
-      <c r="D210" s="63" t="s">
-        <v>152</v>
-      </c>
+      <c r="D210" s="63"/>
       <c r="E210" s="64"/>
       <c r="F210" s="65"/>
     </row>
     <row r="211" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B211" s="61" t="s">
-        <v>153</v>
+        <v>91</v>
       </c>
       <c r="C211" s="62"/>
-      <c r="D211" s="63">
-        <v>1998</v>
-      </c>
+      <c r="D211" s="63"/>
       <c r="E211" s="64"/>
       <c r="F211" s="65"/>
     </row>
     <row r="212" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B212" s="61" t="s">
-        <v>154</v>
+        <v>92</v>
       </c>
       <c r="C212" s="62"/>
-      <c r="D212" s="63">
-        <v>26</v>
-      </c>
+      <c r="D212" s="63"/>
       <c r="E212" s="64"/>
       <c r="F212" s="65"/>
     </row>
     <row r="213" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B213" s="61" t="s">
-        <v>155</v>
+        <v>93</v>
       </c>
       <c r="C213" s="62"/>
-      <c r="D213" s="63" t="s">
-        <v>156</v>
-      </c>
+      <c r="D213" s="63"/>
       <c r="E213" s="64"/>
       <c r="F213" s="65"/>
     </row>
     <row r="214" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B214" s="61" t="s">
-        <v>157</v>
+        <v>94</v>
       </c>
       <c r="C214" s="62"/>
-      <c r="D214" s="63" t="s">
-        <v>158</v>
-      </c>
+      <c r="D214" s="63"/>
       <c r="E214" s="64"/>
       <c r="F214" s="65"/>
     </row>
@@ -4455,12 +3710,12 @@
     </row>
     <row r="225" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B225" s="10" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
     </row>
     <row r="226" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B226" s="61" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="C226" s="62"/>
       <c r="D226" s="63"/>
@@ -4518,23 +3773,21 @@
     </row>
     <row r="235" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B235" s="10" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
     </row>
     <row r="236" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B236" s="61" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="C236" s="62"/>
-      <c r="D236" s="63" t="s">
-        <v>161</v>
-      </c>
+      <c r="D236" s="63"/>
       <c r="E236" s="64"/>
       <c r="F236" s="65"/>
     </row>
     <row r="237" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B237" s="61" t="s">
-        <v>162</v>
+        <v>97</v>
       </c>
       <c r="C237" s="62"/>
       <c r="D237" s="63"/>
@@ -4592,7 +3845,7 @@
     </row>
     <row r="245" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B245" s="61" t="s">
-        <v>163</v>
+        <v>98</v>
       </c>
       <c r="C245" s="62"/>
       <c r="D245" s="63"/>
@@ -4601,17 +3854,15 @@
     </row>
     <row r="248" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B248" s="10" t="s">
-        <v>164</v>
+        <v>99</v>
       </c>
     </row>
     <row r="249" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B249" s="61" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="C249" s="62"/>
-      <c r="D249" s="63" t="s">
-        <v>165</v>
-      </c>
+      <c r="D249" s="63"/>
       <c r="E249" s="64"/>
       <c r="F249" s="65"/>
     </row>
@@ -4666,17 +3917,15 @@
     </row>
     <row r="258" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B258" s="10" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
     </row>
     <row r="259" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B259" s="61" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="C259" s="62"/>
-      <c r="D259" s="63" t="s">
-        <v>167</v>
-      </c>
+      <c r="D259" s="63"/>
       <c r="E259" s="64"/>
       <c r="F259" s="65"/>
     </row>
@@ -4731,28 +3980,24 @@
     </row>
     <row r="268" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="9" t="s">
-        <v>168</v>
+        <v>101</v>
       </c>
     </row>
     <row r="269" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B269" s="61" t="s">
-        <v>169</v>
+        <v>102</v>
       </c>
       <c r="C269" s="62"/>
-      <c r="D269" s="63">
-        <v>6</v>
-      </c>
+      <c r="D269" s="63"/>
       <c r="E269" s="64"/>
       <c r="F269" s="65"/>
     </row>
     <row r="270" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B270" s="61" t="s">
-        <v>170</v>
+        <v>103</v>
       </c>
       <c r="C270" s="62"/>
-      <c r="D270" s="63" t="s">
-        <v>171</v>
-      </c>
+      <c r="D270" s="63"/>
       <c r="E270" s="64"/>
       <c r="F270" s="65"/>
     </row>
@@ -4807,329 +4052,193 @@
     </row>
     <row r="281" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" s="9" t="s">
-        <v>172</v>
+        <v>104</v>
       </c>
     </row>
     <row r="283" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" s="18" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B283" s="18" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C283" s="19" t="s">
-        <v>173</v>
+        <v>105</v>
       </c>
       <c r="D283" s="60" t="s">
-        <v>174</v>
+        <v>106</v>
       </c>
       <c r="E283" s="60"/>
       <c r="F283" s="20" t="s">
-        <v>175</v>
+        <v>107</v>
       </c>
       <c r="G283" s="20" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="284" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B284" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C284" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="D284" s="58">
-        <v>2.5</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B284" s="21"/>
+      <c r="C284" s="22"/>
+      <c r="D284" s="58"/>
       <c r="E284" s="59"/>
-      <c r="F284" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="G284" s="21">
-        <v>9.86</v>
-      </c>
+      <c r="F284" s="21"/>
+      <c r="G284" s="21"/>
     </row>
     <row r="285" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A285" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B285" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C285" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="D285" s="58">
-        <v>2.5</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B285" s="21"/>
+      <c r="C285" s="22"/>
+      <c r="D285" s="58"/>
       <c r="E285" s="59"/>
-      <c r="F285" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="G285" s="21">
-        <v>9.4700000000000006</v>
-      </c>
+      <c r="F285" s="21"/>
+      <c r="G285" s="21"/>
     </row>
     <row r="286" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B286" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C286" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="D286" s="58">
-        <v>2.5</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B286" s="21"/>
+      <c r="C286" s="22"/>
+      <c r="D286" s="58"/>
       <c r="E286" s="59"/>
-      <c r="F286" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="G286" s="21">
-        <v>1.35</v>
-      </c>
+      <c r="F286" s="21"/>
+      <c r="G286" s="21"/>
     </row>
     <row r="287" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A287" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B287" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C287" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="D287" s="58" t="s">
-        <v>180</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B287" s="21"/>
+      <c r="C287" s="22"/>
+      <c r="D287" s="58"/>
       <c r="E287" s="59"/>
-      <c r="F287" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="G287" s="21">
-        <v>4.42</v>
-      </c>
+      <c r="F287" s="21"/>
+      <c r="G287" s="21"/>
     </row>
     <row r="288" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B288" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C288" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="D288" s="58">
-        <v>2.5</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B288" s="21"/>
+      <c r="C288" s="22"/>
+      <c r="D288" s="58"/>
       <c r="E288" s="59"/>
-      <c r="F288" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="G288" s="21">
-        <v>29.11</v>
-      </c>
+      <c r="F288" s="21"/>
+      <c r="G288" s="21"/>
     </row>
     <row r="289" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A289" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B289" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C289" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="D289" s="58">
-        <v>2.5</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B289" s="21"/>
+      <c r="C289" s="22"/>
+      <c r="D289" s="58"/>
       <c r="E289" s="59"/>
-      <c r="F289" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="G289" s="21">
-        <v>7.97</v>
-      </c>
+      <c r="F289" s="21"/>
+      <c r="G289" s="21"/>
     </row>
     <row r="290" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A290" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B290" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C290" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="D290" s="58">
-        <v>2.5</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B290" s="21"/>
+      <c r="C290" s="22"/>
+      <c r="D290" s="58"/>
       <c r="E290" s="59"/>
-      <c r="F290" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="G290" s="21">
-        <v>4.93</v>
-      </c>
+      <c r="F290" s="21"/>
+      <c r="G290" s="21"/>
     </row>
     <row r="291" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A291" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B291" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C291" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="D291" s="58">
-        <v>2.5</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B291" s="21"/>
+      <c r="C291" s="22"/>
+      <c r="D291" s="58"/>
       <c r="E291" s="59"/>
-      <c r="F291" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="G291" s="21">
-        <v>12.71</v>
-      </c>
+      <c r="F291" s="21"/>
+      <c r="G291" s="21"/>
     </row>
     <row r="292" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A292" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="B292" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C292" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="D292" s="58">
-        <v>2.5</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B292" s="21"/>
+      <c r="C292" s="22"/>
+      <c r="D292" s="58"/>
       <c r="E292" s="59"/>
-      <c r="F292" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="G292" s="21">
-        <v>11.39</v>
-      </c>
+      <c r="F292" s="21"/>
+      <c r="G292" s="21"/>
     </row>
     <row r="293" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B293" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C293" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="D293" s="58">
-        <v>2.5</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B293" s="21"/>
+      <c r="C293" s="22"/>
+      <c r="D293" s="58"/>
       <c r="E293" s="59"/>
-      <c r="F293" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="G293" s="21">
-        <v>12.53</v>
-      </c>
+      <c r="F293" s="21"/>
+      <c r="G293" s="21"/>
     </row>
     <row r="294" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A294" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B294" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C294" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="D294" s="58">
-        <v>2.5</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B294" s="21"/>
+      <c r="C294" s="22"/>
+      <c r="D294" s="58"/>
       <c r="E294" s="59"/>
-      <c r="F294" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="G294" s="21">
-        <v>1.37</v>
-      </c>
+      <c r="F294" s="21"/>
+      <c r="G294" s="21"/>
     </row>
     <row r="295" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A295" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="B295" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C295" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="D295" s="58">
-        <v>2.5</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B295" s="21"/>
+      <c r="C295" s="22"/>
+      <c r="D295" s="58"/>
       <c r="E295" s="59"/>
-      <c r="F295" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="G295" s="21">
-        <v>3.68</v>
-      </c>
+      <c r="F295" s="21"/>
+      <c r="G295" s="21"/>
     </row>
     <row r="296" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A296" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B296" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C296" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="D296" s="58">
-        <v>2.5</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B296" s="21"/>
+      <c r="C296" s="22"/>
+      <c r="D296" s="58"/>
       <c r="E296" s="59"/>
-      <c r="F296" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="G296" s="21">
-        <v>0</v>
-      </c>
+      <c r="F296" s="21"/>
+      <c r="G296" s="21"/>
     </row>
     <row r="297" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A297" s="21"/>
-      <c r="B297" s="21" t="s">
-        <v>47</v>
-      </c>
+      <c r="B297" s="21"/>
       <c r="C297" s="22"/>
       <c r="D297" s="58" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
       <c r="E297" s="59"/>
-      <c r="F297" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="G297" s="21">
-        <v>0</v>
-      </c>
+      <c r="F297" s="21"/>
+      <c r="G297" s="21"/>
     </row>
     <row r="342" spans="1:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="344" spans="1:6" ht="30.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A344" s="9" t="s">
-        <v>194</v>
+        <v>109</v>
       </c>
     </row>
     <row r="345" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B345" s="66" t="s">
-        <v>195</v>
+        <v>110</v>
       </c>
       <c r="C345" s="66"/>
       <c r="D345" s="66"/>
@@ -5138,7 +4247,7 @@
     </row>
     <row r="347" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B347" s="52" t="s">
-        <v>196</v>
+        <v>111</v>
       </c>
       <c r="C347" s="53"/>
       <c r="D347" s="53"/>
@@ -5161,7 +4270,7 @@
     </row>
     <row r="352" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B352" s="52" t="s">
-        <v>197</v>
+        <v>112</v>
       </c>
       <c r="C352" s="53"/>
       <c r="D352" s="53"/>

</xml_diff>